<commit_message>
add mutiple b_localDebug flag in different function
</commit_message>
<xml_diff>
--- a/Auto_RRSIandWiFiSAR_Report/output/WillyWJ_Chen/RSSI.xlsx
+++ b/Auto_RRSIandWiFiSAR_Report/output/WillyWJ_Chen/RSSI.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="RSSI" sheetId="1" state="visible" r:id="rId1"/>
@@ -52,16 +52,16 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -605,12 +605,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="7"/>
-    <col customWidth="1" max="2" min="2" width="16"/>
-    <col customWidth="1" max="3" min="3" width="14"/>
-    <col customWidth="1" max="4" min="4" width="7"/>
-    <col customWidth="1" max="5" min="5" width="6"/>
-    <col customWidth="1" max="6" min="6" width="7"/>
+    <col width="7" customWidth="1" min="1" max="1"/>
+    <col width="16" customWidth="1" min="2" max="2"/>
+    <col width="14" customWidth="1" min="3" max="3"/>
+    <col width="7" customWidth="1" min="4" max="4"/>
+    <col width="6" customWidth="1" min="5" max="5"/>
+    <col width="7" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -651,7 +651,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>7224908800005</t>
+          <t>7228124300036</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -660,10 +660,10 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>-61</v>
+        <v>-46</v>
       </c>
       <c r="E2" t="n">
-        <v>-62</v>
+        <v>-48</v>
       </c>
       <c r="F2" t="n">
         <v>-65</v>
@@ -675,7 +675,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>7224908800006</t>
+          <t>7228124300026</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -684,10 +684,10 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>-62</v>
+        <v>-61</v>
       </c>
       <c r="E3" t="n">
-        <v>-60</v>
+        <v>-58</v>
       </c>
       <c r="F3" t="n">
         <v>-65</v>
@@ -699,7 +699,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>7224908800007</t>
+          <t>7228124200065</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -708,10 +708,10 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>-60</v>
+        <v>-47</v>
       </c>
       <c r="E4" t="n">
-        <v>-60</v>
+        <v>-54</v>
       </c>
       <c r="F4" t="n">
         <v>-65</v>
@@ -723,7 +723,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>7228101300001</t>
+          <t>7228979800008</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -732,10 +732,10 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>-60</v>
+        <v>-55</v>
       </c>
       <c r="E5" t="n">
-        <v>-63</v>
+        <v>-51</v>
       </c>
       <c r="F5" t="n">
         <v>-65</v>
@@ -747,7 +747,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>7228101400001</t>
+          <t>7228124200054</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -756,10 +756,10 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>-55</v>
+        <v>-47</v>
       </c>
       <c r="E6" t="n">
-        <v>-58</v>
+        <v>-45</v>
       </c>
       <c r="F6" t="n">
         <v>-65</v>
@@ -771,7 +771,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>7228101600001</t>
+          <t>7228124200012</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -780,7 +780,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>-60</v>
+        <v>-50</v>
       </c>
       <c r="E7" t="n">
         <v>-54</v>
@@ -795,7 +795,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>7228101700001</t>
+          <t>7228124300034</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -804,10 +804,10 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>-53</v>
+        <v>-40</v>
       </c>
       <c r="E8" t="n">
-        <v>-59</v>
+        <v>-55</v>
       </c>
       <c r="F8" t="n">
         <v>-65</v>
@@ -819,7 +819,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>7228101900001</t>
+          <t>7228124200036</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -828,10 +828,10 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>-50</v>
+        <v>-53</v>
       </c>
       <c r="E9" t="n">
-        <v>-59</v>
+        <v>-57</v>
       </c>
       <c r="F9" t="n">
         <v>-65</v>
@@ -843,7 +843,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>7228124100001</t>
+          <t>7228124300076</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -852,10 +852,10 @@
         </is>
       </c>
       <c r="D10" t="n">
+        <v>-56</v>
+      </c>
+      <c r="E10" t="n">
         <v>-54</v>
-      </c>
-      <c r="E10" t="n">
-        <v>-63</v>
       </c>
       <c r="F10" t="n">
         <v>-65</v>
@@ -867,7 +867,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>7228124200002</t>
+          <t>7228124300006</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -876,10 +876,10 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>-61</v>
+        <v>-51</v>
       </c>
       <c r="E11" t="n">
-        <v>-65</v>
+        <v>-56</v>
       </c>
       <c r="F11" t="n">
         <v>-65</v>
@@ -891,7 +891,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>7228124200003</t>
+          <t>7228124200006</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -900,10 +900,10 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>-50</v>
+        <v>-60</v>
       </c>
       <c r="E12" t="n">
-        <v>-46</v>
+        <v>-65</v>
       </c>
       <c r="F12" t="n">
         <v>-65</v>
@@ -915,7 +915,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>7228124200004</t>
+          <t>7228124300012</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -924,10 +924,10 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>-49</v>
+        <v>-53</v>
       </c>
       <c r="E13" t="n">
-        <v>-55</v>
+        <v>-50</v>
       </c>
       <c r="F13" t="n">
         <v>-65</v>
@@ -939,7 +939,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>7228124200005</t>
+          <t>7228124200010</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -948,7 +948,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>-58</v>
+        <v>-47</v>
       </c>
       <c r="E14" t="n">
         <v>-58</v>
@@ -963,7 +963,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>7228124200006</t>
+          <t>7228124200029</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -972,10 +972,10 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>-60</v>
+        <v>-51</v>
       </c>
       <c r="E15" t="n">
-        <v>-65</v>
+        <v>-40</v>
       </c>
       <c r="F15" t="n">
         <v>-65</v>
@@ -987,7 +987,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>7228124200007</t>
+          <t>7228124200025</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -996,10 +996,10 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>-59</v>
+        <v>-57</v>
       </c>
       <c r="E16" t="n">
-        <v>-58</v>
+        <v>-63</v>
       </c>
       <c r="F16" t="n">
         <v>-65</v>
@@ -1011,7 +1011,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>7228124200008</t>
+          <t>7228124300010</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1020,10 +1020,10 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>-63</v>
+        <v>-47</v>
       </c>
       <c r="E17" t="n">
-        <v>-62</v>
+        <v>-55</v>
       </c>
       <c r="F17" t="n">
         <v>-65</v>
@@ -1035,7 +1035,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>7228124200010</t>
+          <t>7228124300077</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1044,10 +1044,10 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>-47</v>
+        <v>-54</v>
       </c>
       <c r="E18" t="n">
-        <v>-58</v>
+        <v>-52</v>
       </c>
       <c r="F18" t="n">
         <v>-65</v>
@@ -1059,7 +1059,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>7228124200012</t>
+          <t>7228124300074</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1068,10 +1068,10 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>-50</v>
+        <v>-52</v>
       </c>
       <c r="E19" t="n">
-        <v>-54</v>
+        <v>-57</v>
       </c>
       <c r="F19" t="n">
         <v>-65</v>
@@ -1083,7 +1083,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>7228124200013</t>
+          <t>7228124300081</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1092,10 +1092,10 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>-43</v>
+        <v>-59</v>
       </c>
       <c r="E20" t="n">
-        <v>-49</v>
+        <v>-60</v>
       </c>
       <c r="F20" t="n">
         <v>-65</v>
@@ -1107,7 +1107,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>7228124200014</t>
+          <t>7228124200033</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1116,10 +1116,10 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>-49</v>
+        <v>-40</v>
       </c>
       <c r="E21" t="n">
-        <v>-48</v>
+        <v>-41</v>
       </c>
       <c r="F21" t="n">
         <v>-65</v>
@@ -1131,7 +1131,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>7228124200017</t>
+          <t>7228124300050</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1140,10 +1140,10 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>-59</v>
+        <v>-56</v>
       </c>
       <c r="E22" t="n">
-        <v>-57</v>
+        <v>-63</v>
       </c>
       <c r="F22" t="n">
         <v>-65</v>
@@ -1155,7 +1155,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>7228124200018</t>
+          <t>7228124300067</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1167,7 +1167,7 @@
         <v>-59</v>
       </c>
       <c r="E23" t="n">
-        <v>-60</v>
+        <v>-58</v>
       </c>
       <c r="F23" t="n">
         <v>-65</v>
@@ -1179,7 +1179,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>7228124200019</t>
+          <t>7228124300058</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1188,10 +1188,10 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>-53</v>
+        <v>-57</v>
       </c>
       <c r="E24" t="n">
-        <v>-50</v>
+        <v>-60</v>
       </c>
       <c r="F24" t="n">
         <v>-65</v>
@@ -1203,7 +1203,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>7228124200020</t>
+          <t>7228125100001</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1212,10 +1212,10 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>-53</v>
+        <v>-56</v>
       </c>
       <c r="E25" t="n">
-        <v>-50</v>
+        <v>-59</v>
       </c>
       <c r="F25" t="n">
         <v>-65</v>
@@ -1227,7 +1227,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>7228124200021</t>
+          <t>7228124300011</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1236,10 +1236,10 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>-65</v>
+        <v>-44</v>
       </c>
       <c r="E26" t="n">
-        <v>-65</v>
+        <v>-41</v>
       </c>
       <c r="F26" t="n">
         <v>-65</v>
@@ -1251,7 +1251,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>7228124200022</t>
+          <t>7228124200043</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1260,10 +1260,10 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>-57</v>
+        <v>-59</v>
       </c>
       <c r="E27" t="n">
-        <v>-50</v>
+        <v>-64</v>
       </c>
       <c r="F27" t="n">
         <v>-65</v>
@@ -1275,7 +1275,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>7228124200023</t>
+          <t>7228124200008</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1284,10 +1284,10 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>-54</v>
+        <v>-63</v>
       </c>
       <c r="E28" t="n">
-        <v>-49</v>
+        <v>-62</v>
       </c>
       <c r="F28" t="n">
         <v>-65</v>
@@ -1299,7 +1299,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>7228124200024</t>
+          <t>7228124200003</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1308,10 +1308,10 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>-59</v>
+        <v>-50</v>
       </c>
       <c r="E29" t="n">
-        <v>-55</v>
+        <v>-46</v>
       </c>
       <c r="F29" t="n">
         <v>-65</v>
@@ -1323,7 +1323,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>7228124200025</t>
+          <t>7228124200060</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1335,7 +1335,7 @@
         <v>-57</v>
       </c>
       <c r="E30" t="n">
-        <v>-63</v>
+        <v>-56</v>
       </c>
       <c r="F30" t="n">
         <v>-65</v>
@@ -1347,7 +1347,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>7228124200026</t>
+          <t>7228101900001</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1356,10 +1356,10 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>-55</v>
+        <v>-50</v>
       </c>
       <c r="E31" t="n">
-        <v>-60</v>
+        <v>-59</v>
       </c>
       <c r="F31" t="n">
         <v>-65</v>
@@ -1371,7 +1371,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>7228124200027</t>
+          <t>7228124200059</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1380,10 +1380,10 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>-65</v>
+        <v>-50</v>
       </c>
       <c r="E32" t="n">
-        <v>-59</v>
+        <v>-56</v>
       </c>
       <c r="F32" t="n">
         <v>-65</v>
@@ -1419,7 +1419,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>7228124200029</t>
+          <t>7228124200038</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1428,10 +1428,10 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>-51</v>
+        <v>-57</v>
       </c>
       <c r="E34" t="n">
-        <v>-40</v>
+        <v>-59</v>
       </c>
       <c r="F34" t="n">
         <v>-65</v>
@@ -1443,7 +1443,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>7228124200030</t>
+          <t>7228124300009</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1452,10 +1452,10 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>-58</v>
+        <v>-64</v>
       </c>
       <c r="E35" t="n">
-        <v>-61</v>
+        <v>-64</v>
       </c>
       <c r="F35" t="n">
         <v>-65</v>
@@ -1467,7 +1467,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>7228124200031</t>
+          <t>7228124300053</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1476,10 +1476,10 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>-53</v>
+        <v>-52</v>
       </c>
       <c r="E36" t="n">
-        <v>-50</v>
+        <v>-62</v>
       </c>
       <c r="F36" t="n">
         <v>-65</v>
@@ -1491,7 +1491,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>7228124200033</t>
+          <t>7228124300084</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1500,10 +1500,10 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>-40</v>
+        <v>-57</v>
       </c>
       <c r="E37" t="n">
-        <v>-41</v>
+        <v>-62</v>
       </c>
       <c r="F37" t="n">
         <v>-65</v>
@@ -1515,7 +1515,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>7228124200034</t>
+          <t>7228124200039</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1524,10 +1524,10 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>-60</v>
+        <v>-56</v>
       </c>
       <c r="E38" t="n">
-        <v>-63</v>
+        <v>-65</v>
       </c>
       <c r="F38" t="n">
         <v>-65</v>
@@ -1539,7 +1539,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>7228124200035</t>
+          <t>7228124200018</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1548,7 +1548,7 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>-65</v>
+        <v>-59</v>
       </c>
       <c r="E39" t="n">
         <v>-60</v>
@@ -1563,7 +1563,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>7228124200036</t>
+          <t>7228124200002</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1572,10 +1572,10 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>-53</v>
+        <v>-61</v>
       </c>
       <c r="E40" t="n">
-        <v>-57</v>
+        <v>-65</v>
       </c>
       <c r="F40" t="n">
         <v>-65</v>
@@ -1587,7 +1587,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>7228124200037</t>
+          <t>7228124200019</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1596,10 +1596,10 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>-41</v>
+        <v>-53</v>
       </c>
       <c r="E41" t="n">
-        <v>-59</v>
+        <v>-50</v>
       </c>
       <c r="F41" t="n">
         <v>-65</v>
@@ -1611,7 +1611,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>7228124200038</t>
+          <t>7228124200067</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1620,10 +1620,10 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>-57</v>
+        <v>-61</v>
       </c>
       <c r="E42" t="n">
-        <v>-59</v>
+        <v>-61</v>
       </c>
       <c r="F42" t="n">
         <v>-65</v>
@@ -1635,7 +1635,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>7228124200039</t>
+          <t>7228124300069</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1644,10 +1644,10 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>-56</v>
+        <v>-54</v>
       </c>
       <c r="E43" t="n">
-        <v>-65</v>
+        <v>-59</v>
       </c>
       <c r="F43" t="n">
         <v>-65</v>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>7228124200040</t>
+          <t>7228124200004</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1668,10 +1668,10 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>-62</v>
+        <v>-49</v>
       </c>
       <c r="E44" t="n">
-        <v>-64</v>
+        <v>-55</v>
       </c>
       <c r="F44" t="n">
         <v>-65</v>
@@ -1683,7 +1683,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>7228124200041</t>
+          <t>7228124300033</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1692,10 +1692,10 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>-49</v>
+        <v>-60</v>
       </c>
       <c r="E45" t="n">
-        <v>-53</v>
+        <v>-60</v>
       </c>
       <c r="F45" t="n">
         <v>-65</v>
@@ -1707,7 +1707,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>7228124200042</t>
+          <t>7228124300035</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1716,10 +1716,10 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>-60</v>
+        <v>-45</v>
       </c>
       <c r="E46" t="n">
-        <v>-60</v>
+        <v>-57</v>
       </c>
       <c r="F46" t="n">
         <v>-65</v>
@@ -1731,7 +1731,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>7228124200043</t>
+          <t>7228124300016</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1740,10 +1740,10 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>-59</v>
+        <v>-60</v>
       </c>
       <c r="E47" t="n">
-        <v>-64</v>
+        <v>-62</v>
       </c>
       <c r="F47" t="n">
         <v>-65</v>
@@ -1755,7 +1755,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>7228124200044</t>
+          <t>7228124200040</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1764,10 +1764,10 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>-55</v>
+        <v>-62</v>
       </c>
       <c r="E48" t="n">
-        <v>-46</v>
+        <v>-64</v>
       </c>
       <c r="F48" t="n">
         <v>-65</v>
@@ -1779,7 +1779,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>7228124200045</t>
+          <t>7224908800005</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1788,10 +1788,10 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>-40</v>
+        <v>-61</v>
       </c>
       <c r="E49" t="n">
-        <v>-53</v>
+        <v>-62</v>
       </c>
       <c r="F49" t="n">
         <v>-65</v>
@@ -1803,7 +1803,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>7228124200046</t>
+          <t>7228124200042</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1812,10 +1812,10 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>-61</v>
+        <v>-60</v>
       </c>
       <c r="E50" t="n">
-        <v>-65</v>
+        <v>-60</v>
       </c>
       <c r="F50" t="n">
         <v>-65</v>
@@ -1827,7 +1827,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>7228124200047</t>
+          <t>7228124300028</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1836,10 +1836,10 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>-50</v>
+        <v>-65</v>
       </c>
       <c r="E51" t="n">
-        <v>-47</v>
+        <v>-61</v>
       </c>
       <c r="F51" t="n">
         <v>-65</v>
@@ -1851,7 +1851,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>7228124200048</t>
+          <t>7228124200052</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1860,10 +1860,10 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>-49</v>
+        <v>-64</v>
       </c>
       <c r="E52" t="n">
-        <v>-52</v>
+        <v>-58</v>
       </c>
       <c r="F52" t="n">
         <v>-65</v>
@@ -1875,7 +1875,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>7228124200049</t>
+          <t>7228124300057</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1884,10 +1884,10 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>-62</v>
+        <v>-41</v>
       </c>
       <c r="E53" t="n">
-        <v>-58</v>
+        <v>-43</v>
       </c>
       <c r="F53" t="n">
         <v>-65</v>
@@ -1923,7 +1923,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>7228124200052</t>
+          <t>7228124200037</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -1932,10 +1932,10 @@
         </is>
       </c>
       <c r="D55" t="n">
-        <v>-64</v>
+        <v>-41</v>
       </c>
       <c r="E55" t="n">
-        <v>-58</v>
+        <v>-59</v>
       </c>
       <c r="F55" t="n">
         <v>-65</v>
@@ -1947,7 +1947,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>7228124200053</t>
+          <t>7228124200076</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -1956,10 +1956,10 @@
         </is>
       </c>
       <c r="D56" t="n">
-        <v>-58</v>
+        <v>-62</v>
       </c>
       <c r="E56" t="n">
-        <v>-61</v>
+        <v>-64</v>
       </c>
       <c r="F56" t="n">
         <v>-65</v>
@@ -1971,7 +1971,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>7228124200054</t>
+          <t>7228124200084</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -1980,10 +1980,10 @@
         </is>
       </c>
       <c r="D57" t="n">
-        <v>-47</v>
+        <v>-38</v>
       </c>
       <c r="E57" t="n">
-        <v>-45</v>
+        <v>-48</v>
       </c>
       <c r="F57" t="n">
         <v>-65</v>
@@ -1995,7 +1995,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>7228124200055</t>
+          <t>7228101600001</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2007,7 +2007,7 @@
         <v>-60</v>
       </c>
       <c r="E58" t="n">
-        <v>-59</v>
+        <v>-54</v>
       </c>
       <c r="F58" t="n">
         <v>-65</v>
@@ -2019,7 +2019,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>7228124200056</t>
+          <t>7228124300032</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -2028,10 +2028,10 @@
         </is>
       </c>
       <c r="D59" t="n">
-        <v>-65</v>
+        <v>-53</v>
       </c>
       <c r="E59" t="n">
-        <v>-62</v>
+        <v>-52</v>
       </c>
       <c r="F59" t="n">
         <v>-65</v>
@@ -2043,7 +2043,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>7228124200057</t>
+          <t>7228124200005</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2052,10 +2052,10 @@
         </is>
       </c>
       <c r="D60" t="n">
-        <v>-55</v>
+        <v>-58</v>
       </c>
       <c r="E60" t="n">
-        <v>-57</v>
+        <v>-58</v>
       </c>
       <c r="F60" t="n">
         <v>-65</v>
@@ -2067,7 +2067,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>7228124200058</t>
+          <t>7228124200062</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2076,10 +2076,10 @@
         </is>
       </c>
       <c r="D61" t="n">
-        <v>-57</v>
+        <v>-53</v>
       </c>
       <c r="E61" t="n">
-        <v>-62</v>
+        <v>-53</v>
       </c>
       <c r="F61" t="n">
         <v>-65</v>
@@ -2091,7 +2091,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>7228124200059</t>
+          <t>7228124200014</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2100,10 +2100,10 @@
         </is>
       </c>
       <c r="D62" t="n">
-        <v>-50</v>
+        <v>-49</v>
       </c>
       <c r="E62" t="n">
-        <v>-56</v>
+        <v>-48</v>
       </c>
       <c r="F62" t="n">
         <v>-65</v>
@@ -2115,7 +2115,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>7228124200060</t>
+          <t>7228124200080</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -2124,10 +2124,10 @@
         </is>
       </c>
       <c r="D63" t="n">
-        <v>-57</v>
+        <v>-60</v>
       </c>
       <c r="E63" t="n">
-        <v>-56</v>
+        <v>-62</v>
       </c>
       <c r="F63" t="n">
         <v>-65</v>
@@ -2139,7 +2139,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>7228124200061</t>
+          <t>7228124200057</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -2148,10 +2148,10 @@
         </is>
       </c>
       <c r="D64" t="n">
-        <v>-51</v>
+        <v>-55</v>
       </c>
       <c r="E64" t="n">
-        <v>-60</v>
+        <v>-57</v>
       </c>
       <c r="F64" t="n">
         <v>-65</v>
@@ -2163,7 +2163,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>7228124200062</t>
+          <t>7228124300063</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -2172,10 +2172,10 @@
         </is>
       </c>
       <c r="D65" t="n">
-        <v>-53</v>
+        <v>-48</v>
       </c>
       <c r="E65" t="n">
-        <v>-53</v>
+        <v>-55</v>
       </c>
       <c r="F65" t="n">
         <v>-65</v>
@@ -2187,7 +2187,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>7228124200064</t>
+          <t>7228124200077</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2196,10 +2196,10 @@
         </is>
       </c>
       <c r="D66" t="n">
-        <v>-56</v>
+        <v>-61</v>
       </c>
       <c r="E66" t="n">
-        <v>-54</v>
+        <v>-57</v>
       </c>
       <c r="F66" t="n">
         <v>-65</v>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>7228124200065</t>
+          <t>7228124200048</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2220,10 +2220,10 @@
         </is>
       </c>
       <c r="D67" t="n">
-        <v>-47</v>
+        <v>-49</v>
       </c>
       <c r="E67" t="n">
-        <v>-54</v>
+        <v>-52</v>
       </c>
       <c r="F67" t="n">
         <v>-65</v>
@@ -2235,7 +2235,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>7228124200066</t>
+          <t>7228124300030</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -2244,10 +2244,10 @@
         </is>
       </c>
       <c r="D68" t="n">
-        <v>-59</v>
+        <v>-48</v>
       </c>
       <c r="E68" t="n">
-        <v>-56</v>
+        <v>-51</v>
       </c>
       <c r="F68" t="n">
         <v>-65</v>
@@ -2259,7 +2259,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>7228124200067</t>
+          <t>7228124300062</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -2268,10 +2268,10 @@
         </is>
       </c>
       <c r="D69" t="n">
-        <v>-61</v>
+        <v>-54</v>
       </c>
       <c r="E69" t="n">
-        <v>-61</v>
+        <v>-49</v>
       </c>
       <c r="F69" t="n">
         <v>-65</v>
@@ -2283,7 +2283,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>7228124200068</t>
+          <t>7228101300001</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -2292,10 +2292,10 @@
         </is>
       </c>
       <c r="D70" t="n">
-        <v>-56</v>
+        <v>-60</v>
       </c>
       <c r="E70" t="n">
-        <v>-51</v>
+        <v>-63</v>
       </c>
       <c r="F70" t="n">
         <v>-65</v>
@@ -2307,7 +2307,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>7228124200069</t>
+          <t>7228124200066</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -2316,10 +2316,10 @@
         </is>
       </c>
       <c r="D71" t="n">
-        <v>-54</v>
+        <v>-59</v>
       </c>
       <c r="E71" t="n">
-        <v>-55</v>
+        <v>-56</v>
       </c>
       <c r="F71" t="n">
         <v>-65</v>
@@ -2331,7 +2331,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>7228124200070</t>
+          <t>7228124200082</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -2340,7 +2340,7 @@
         </is>
       </c>
       <c r="D72" t="n">
-        <v>-61</v>
+        <v>-63</v>
       </c>
       <c r="E72" t="n">
         <v>-63</v>
@@ -2355,7 +2355,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>7228124200071</t>
+          <t>7228124200020</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -2364,10 +2364,10 @@
         </is>
       </c>
       <c r="D73" t="n">
-        <v>-51</v>
+        <v>-53</v>
       </c>
       <c r="E73" t="n">
-        <v>-53</v>
+        <v>-50</v>
       </c>
       <c r="F73" t="n">
         <v>-65</v>
@@ -2379,7 +2379,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>7228124200075</t>
+          <t>7228124200044</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -2388,10 +2388,10 @@
         </is>
       </c>
       <c r="D74" t="n">
-        <v>-58</v>
+        <v>-55</v>
       </c>
       <c r="E74" t="n">
-        <v>-56</v>
+        <v>-46</v>
       </c>
       <c r="F74" t="n">
         <v>-65</v>
@@ -2403,7 +2403,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>7228124200076</t>
+          <t>7228124300024</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -2412,10 +2412,10 @@
         </is>
       </c>
       <c r="D75" t="n">
-        <v>-62</v>
+        <v>-59</v>
       </c>
       <c r="E75" t="n">
-        <v>-64</v>
+        <v>-57</v>
       </c>
       <c r="F75" t="n">
         <v>-65</v>
@@ -2427,7 +2427,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>7228124200077</t>
+          <t>7228124200021</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -2436,10 +2436,10 @@
         </is>
       </c>
       <c r="D76" t="n">
-        <v>-61</v>
+        <v>-65</v>
       </c>
       <c r="E76" t="n">
-        <v>-57</v>
+        <v>-65</v>
       </c>
       <c r="F76" t="n">
         <v>-65</v>
@@ -2451,7 +2451,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>7228124200078</t>
+          <t>7228124200058</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -2460,10 +2460,10 @@
         </is>
       </c>
       <c r="D77" t="n">
-        <v>-60</v>
+        <v>-57</v>
       </c>
       <c r="E77" t="n">
-        <v>-61</v>
+        <v>-62</v>
       </c>
       <c r="F77" t="n">
         <v>-65</v>
@@ -2475,7 +2475,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>7228124200079</t>
+          <t>7224908800006</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -2484,10 +2484,10 @@
         </is>
       </c>
       <c r="D78" t="n">
-        <v>-64</v>
+        <v>-62</v>
       </c>
       <c r="E78" t="n">
-        <v>-65</v>
+        <v>-60</v>
       </c>
       <c r="F78" t="n">
         <v>-65</v>
@@ -2499,7 +2499,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>7228124200080</t>
+          <t>7228124200068</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -2508,10 +2508,10 @@
         </is>
       </c>
       <c r="D79" t="n">
-        <v>-60</v>
+        <v>-56</v>
       </c>
       <c r="E79" t="n">
-        <v>-62</v>
+        <v>-51</v>
       </c>
       <c r="F79" t="n">
         <v>-65</v>
@@ -2523,7 +2523,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>7228124200081</t>
+          <t>7228124300073</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -2532,10 +2532,10 @@
         </is>
       </c>
       <c r="D80" t="n">
-        <v>-49</v>
+        <v>-55</v>
       </c>
       <c r="E80" t="n">
-        <v>-45</v>
+        <v>-54</v>
       </c>
       <c r="F80" t="n">
         <v>-65</v>
@@ -2547,7 +2547,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>7228124200082</t>
+          <t>7228124200078</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -2556,10 +2556,10 @@
         </is>
       </c>
       <c r="D81" t="n">
-        <v>-63</v>
+        <v>-60</v>
       </c>
       <c r="E81" t="n">
-        <v>-63</v>
+        <v>-61</v>
       </c>
       <c r="F81" t="n">
         <v>-65</v>
@@ -2571,7 +2571,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>7228124200084</t>
+          <t>7228101400001</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -2580,10 +2580,10 @@
         </is>
       </c>
       <c r="D82" t="n">
-        <v>-38</v>
+        <v>-55</v>
       </c>
       <c r="E82" t="n">
-        <v>-48</v>
+        <v>-58</v>
       </c>
       <c r="F82" t="n">
         <v>-65</v>
@@ -2595,7 +2595,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>7228124200085</t>
+          <t>7228124200056</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -2604,10 +2604,10 @@
         </is>
       </c>
       <c r="D83" t="n">
-        <v>-63</v>
+        <v>-65</v>
       </c>
       <c r="E83" t="n">
-        <v>-65</v>
+        <v>-62</v>
       </c>
       <c r="F83" t="n">
         <v>-65</v>
@@ -2619,7 +2619,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>7228124300002</t>
+          <t>7228124200070</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -2628,10 +2628,10 @@
         </is>
       </c>
       <c r="D84" t="n">
-        <v>-43</v>
+        <v>-61</v>
       </c>
       <c r="E84" t="n">
-        <v>-59</v>
+        <v>-63</v>
       </c>
       <c r="F84" t="n">
         <v>-65</v>
@@ -2643,7 +2643,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>7228124300003</t>
+          <t>7228124300025</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -2652,10 +2652,10 @@
         </is>
       </c>
       <c r="D85" t="n">
-        <v>-57</v>
+        <v>-54</v>
       </c>
       <c r="E85" t="n">
-        <v>-58</v>
+        <v>-51</v>
       </c>
       <c r="F85" t="n">
         <v>-65</v>
@@ -2667,7 +2667,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>7228124300006</t>
+          <t>7228124300015</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -2676,10 +2676,10 @@
         </is>
       </c>
       <c r="D86" t="n">
-        <v>-51</v>
+        <v>-64</v>
       </c>
       <c r="E86" t="n">
-        <v>-56</v>
+        <v>-61</v>
       </c>
       <c r="F86" t="n">
         <v>-65</v>
@@ -2691,7 +2691,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>7228124300009</t>
+          <t>7228124200085</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -2700,10 +2700,10 @@
         </is>
       </c>
       <c r="D87" t="n">
-        <v>-64</v>
+        <v>-63</v>
       </c>
       <c r="E87" t="n">
-        <v>-64</v>
+        <v>-65</v>
       </c>
       <c r="F87" t="n">
         <v>-65</v>
@@ -2715,7 +2715,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>7228124300010</t>
+          <t>7224908800007</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -2724,10 +2724,10 @@
         </is>
       </c>
       <c r="D88" t="n">
-        <v>-47</v>
+        <v>-60</v>
       </c>
       <c r="E88" t="n">
-        <v>-55</v>
+        <v>-60</v>
       </c>
       <c r="F88" t="n">
         <v>-65</v>
@@ -2739,7 +2739,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>7228124300011</t>
+          <t>7228124300020</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -2748,10 +2748,10 @@
         </is>
       </c>
       <c r="D89" t="n">
-        <v>-44</v>
+        <v>-51</v>
       </c>
       <c r="E89" t="n">
-        <v>-41</v>
+        <v>-57</v>
       </c>
       <c r="F89" t="n">
         <v>-65</v>
@@ -2763,7 +2763,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>7228124300012</t>
+          <t>7228124300019</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -2772,7 +2772,7 @@
         </is>
       </c>
       <c r="D90" t="n">
-        <v>-53</v>
+        <v>-55</v>
       </c>
       <c r="E90" t="n">
         <v>-50</v>
@@ -2787,7 +2787,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>7228124300013</t>
+          <t>7228124200061</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -2796,10 +2796,10 @@
         </is>
       </c>
       <c r="D91" t="n">
-        <v>-55</v>
+        <v>-51</v>
       </c>
       <c r="E91" t="n">
-        <v>-65</v>
+        <v>-60</v>
       </c>
       <c r="F91" t="n">
         <v>-65</v>
@@ -2811,7 +2811,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>7228124300014</t>
+          <t>7228124300002</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -2820,10 +2820,10 @@
         </is>
       </c>
       <c r="D92" t="n">
-        <v>-64</v>
+        <v>-43</v>
       </c>
       <c r="E92" t="n">
-        <v>-63</v>
+        <v>-59</v>
       </c>
       <c r="F92" t="n">
         <v>-65</v>
@@ -2835,7 +2835,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>7228124300015</t>
+          <t>7228124200041</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -2844,10 +2844,10 @@
         </is>
       </c>
       <c r="D93" t="n">
-        <v>-64</v>
+        <v>-49</v>
       </c>
       <c r="E93" t="n">
-        <v>-61</v>
+        <v>-53</v>
       </c>
       <c r="F93" t="n">
         <v>-65</v>
@@ -2859,7 +2859,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>7228124300016</t>
+          <t>7228124300068</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -2871,7 +2871,7 @@
         <v>-60</v>
       </c>
       <c r="E94" t="n">
-        <v>-62</v>
+        <v>-64</v>
       </c>
       <c r="F94" t="n">
         <v>-65</v>
@@ -2883,7 +2883,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>7228124300018</t>
+          <t>7228124300031</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -2892,10 +2892,10 @@
         </is>
       </c>
       <c r="D95" t="n">
-        <v>-64</v>
+        <v>-53</v>
       </c>
       <c r="E95" t="n">
-        <v>-63</v>
+        <v>-58</v>
       </c>
       <c r="F95" t="n">
         <v>-65</v>
@@ -2907,7 +2907,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>7228124300019</t>
+          <t>7228124300013</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -2919,7 +2919,7 @@
         <v>-55</v>
       </c>
       <c r="E96" t="n">
-        <v>-50</v>
+        <v>-65</v>
       </c>
       <c r="F96" t="n">
         <v>-65</v>
@@ -2931,7 +2931,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>7228124300020</t>
+          <t>7228124300056</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -2940,10 +2940,10 @@
         </is>
       </c>
       <c r="D97" t="n">
-        <v>-51</v>
+        <v>-57</v>
       </c>
       <c r="E97" t="n">
-        <v>-57</v>
+        <v>-55</v>
       </c>
       <c r="F97" t="n">
         <v>-65</v>
@@ -2955,7 +2955,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>7228124300023</t>
+          <t>7228124200035</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -2964,10 +2964,10 @@
         </is>
       </c>
       <c r="D98" t="n">
-        <v>-51</v>
+        <v>-65</v>
       </c>
       <c r="E98" t="n">
-        <v>-51</v>
+        <v>-60</v>
       </c>
       <c r="F98" t="n">
         <v>-65</v>
@@ -2979,7 +2979,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>7228124300024</t>
+          <t>7228979800009</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -2988,10 +2988,10 @@
         </is>
       </c>
       <c r="D99" t="n">
-        <v>-59</v>
+        <v>-56</v>
       </c>
       <c r="E99" t="n">
-        <v>-57</v>
+        <v>-52</v>
       </c>
       <c r="F99" t="n">
         <v>-65</v>
@@ -3003,7 +3003,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>7228124300025</t>
+          <t>7228124300054</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -3012,10 +3012,10 @@
         </is>
       </c>
       <c r="D100" t="n">
-        <v>-54</v>
+        <v>-47</v>
       </c>
       <c r="E100" t="n">
-        <v>-51</v>
+        <v>-52</v>
       </c>
       <c r="F100" t="n">
         <v>-65</v>
@@ -3027,7 +3027,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>7228124300026</t>
+          <t>7228124200031</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -3036,10 +3036,10 @@
         </is>
       </c>
       <c r="D101" t="n">
-        <v>-61</v>
+        <v>-53</v>
       </c>
       <c r="E101" t="n">
-        <v>-58</v>
+        <v>-50</v>
       </c>
       <c r="F101" t="n">
         <v>-65</v>
@@ -3051,7 +3051,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>7228124300028</t>
+          <t>7228124300041</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -3060,10 +3060,10 @@
         </is>
       </c>
       <c r="D102" t="n">
-        <v>-65</v>
+        <v>-57</v>
       </c>
       <c r="E102" t="n">
-        <v>-61</v>
+        <v>-53</v>
       </c>
       <c r="F102" t="n">
         <v>-65</v>
@@ -3075,7 +3075,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>7228124300029</t>
+          <t>7228124200026</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -3084,10 +3084,10 @@
         </is>
       </c>
       <c r="D103" t="n">
-        <v>-57</v>
+        <v>-55</v>
       </c>
       <c r="E103" t="n">
-        <v>-65</v>
+        <v>-60</v>
       </c>
       <c r="F103" t="n">
         <v>-65</v>
@@ -3099,7 +3099,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>7228124300030</t>
+          <t>7228124300039</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -3108,10 +3108,10 @@
         </is>
       </c>
       <c r="D104" t="n">
-        <v>-48</v>
+        <v>-47</v>
       </c>
       <c r="E104" t="n">
-        <v>-51</v>
+        <v>-53</v>
       </c>
       <c r="F104" t="n">
         <v>-65</v>
@@ -3123,7 +3123,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>7228124300031</t>
+          <t>7228124300037</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -3132,10 +3132,10 @@
         </is>
       </c>
       <c r="D105" t="n">
-        <v>-53</v>
+        <v>-56</v>
       </c>
       <c r="E105" t="n">
-        <v>-58</v>
+        <v>-55</v>
       </c>
       <c r="F105" t="n">
         <v>-65</v>
@@ -3147,7 +3147,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>7228124300032</t>
+          <t>7228124300061</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -3159,7 +3159,7 @@
         <v>-53</v>
       </c>
       <c r="E106" t="n">
-        <v>-52</v>
+        <v>-55</v>
       </c>
       <c r="F106" t="n">
         <v>-65</v>
@@ -3171,7 +3171,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>7228124300033</t>
+          <t>7228124200046</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -3180,10 +3180,10 @@
         </is>
       </c>
       <c r="D107" t="n">
-        <v>-60</v>
+        <v>-61</v>
       </c>
       <c r="E107" t="n">
-        <v>-60</v>
+        <v>-65</v>
       </c>
       <c r="F107" t="n">
         <v>-65</v>
@@ -3195,7 +3195,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>7228124300034</t>
+          <t>7228124200075</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -3204,10 +3204,10 @@
         </is>
       </c>
       <c r="D108" t="n">
-        <v>-40</v>
+        <v>-58</v>
       </c>
       <c r="E108" t="n">
-        <v>-55</v>
+        <v>-56</v>
       </c>
       <c r="F108" t="n">
         <v>-65</v>
@@ -3219,7 +3219,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>7228124300035</t>
+          <t>7228124300003</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -3228,10 +3228,10 @@
         </is>
       </c>
       <c r="D109" t="n">
-        <v>-45</v>
+        <v>-57</v>
       </c>
       <c r="E109" t="n">
-        <v>-57</v>
+        <v>-58</v>
       </c>
       <c r="F109" t="n">
         <v>-65</v>
@@ -3243,7 +3243,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>7228124300036</t>
+          <t>7228124300029</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -3252,10 +3252,10 @@
         </is>
       </c>
       <c r="D110" t="n">
-        <v>-46</v>
+        <v>-57</v>
       </c>
       <c r="E110" t="n">
-        <v>-48</v>
+        <v>-65</v>
       </c>
       <c r="F110" t="n">
         <v>-65</v>
@@ -3267,7 +3267,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>7228124300037</t>
+          <t>7228124300082</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -3276,10 +3276,10 @@
         </is>
       </c>
       <c r="D111" t="n">
-        <v>-56</v>
+        <v>-54</v>
       </c>
       <c r="E111" t="n">
-        <v>-55</v>
+        <v>-51</v>
       </c>
       <c r="F111" t="n">
         <v>-65</v>
@@ -3291,7 +3291,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>7228124300038</t>
+          <t>7228124200023</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -3303,7 +3303,7 @@
         <v>-54</v>
       </c>
       <c r="E112" t="n">
-        <v>-55</v>
+        <v>-49</v>
       </c>
       <c r="F112" t="n">
         <v>-65</v>
@@ -3315,7 +3315,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>7228124300039</t>
+          <t>7228124300060</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -3324,10 +3324,10 @@
         </is>
       </c>
       <c r="D113" t="n">
-        <v>-47</v>
+        <v>-62</v>
       </c>
       <c r="E113" t="n">
-        <v>-53</v>
+        <v>-61</v>
       </c>
       <c r="F113" t="n">
         <v>-65</v>
@@ -3339,7 +3339,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>7228124300040</t>
+          <t>7228124200049</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -3351,7 +3351,7 @@
         <v>-62</v>
       </c>
       <c r="E114" t="n">
-        <v>-64</v>
+        <v>-58</v>
       </c>
       <c r="F114" t="n">
         <v>-65</v>
@@ -3363,7 +3363,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>7228124300041</t>
+          <t>7228101700001</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -3372,10 +3372,10 @@
         </is>
       </c>
       <c r="D115" t="n">
-        <v>-57</v>
+        <v>-53</v>
       </c>
       <c r="E115" t="n">
-        <v>-53</v>
+        <v>-59</v>
       </c>
       <c r="F115" t="n">
         <v>-65</v>
@@ -3387,7 +3387,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>7228124300042</t>
+          <t>7228124300023</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -3396,10 +3396,10 @@
         </is>
       </c>
       <c r="D116" t="n">
-        <v>-58</v>
+        <v>-51</v>
       </c>
       <c r="E116" t="n">
-        <v>-61</v>
+        <v>-51</v>
       </c>
       <c r="F116" t="n">
         <v>-65</v>
@@ -3411,7 +3411,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>7228124300045</t>
+          <t>7228124300086</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -3420,10 +3420,10 @@
         </is>
       </c>
       <c r="D117" t="n">
-        <v>-61</v>
+        <v>-50</v>
       </c>
       <c r="E117" t="n">
-        <v>-63</v>
+        <v>-55</v>
       </c>
       <c r="F117" t="n">
         <v>-65</v>
@@ -3435,7 +3435,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>7228124300047</t>
+          <t>7228124300059</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -3444,10 +3444,10 @@
         </is>
       </c>
       <c r="D118" t="n">
-        <v>-55</v>
+        <v>-50</v>
       </c>
       <c r="E118" t="n">
-        <v>-51</v>
+        <v>-54</v>
       </c>
       <c r="F118" t="n">
         <v>-65</v>
@@ -3459,7 +3459,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>7228124300048</t>
+          <t>7228124200079</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -3468,10 +3468,10 @@
         </is>
       </c>
       <c r="D119" t="n">
-        <v>-57</v>
+        <v>-64</v>
       </c>
       <c r="E119" t="n">
-        <v>-59</v>
+        <v>-65</v>
       </c>
       <c r="F119" t="n">
         <v>-65</v>
@@ -3483,7 +3483,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>7228124300049</t>
+          <t>7228124100001</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
@@ -3492,10 +3492,10 @@
         </is>
       </c>
       <c r="D120" t="n">
-        <v>-57</v>
+        <v>-54</v>
       </c>
       <c r="E120" t="n">
-        <v>-62</v>
+        <v>-63</v>
       </c>
       <c r="F120" t="n">
         <v>-65</v>
@@ -3507,7 +3507,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>7228124300050</t>
+          <t>7228124200081</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
@@ -3516,10 +3516,10 @@
         </is>
       </c>
       <c r="D121" t="n">
-        <v>-56</v>
+        <v>-49</v>
       </c>
       <c r="E121" t="n">
-        <v>-63</v>
+        <v>-45</v>
       </c>
       <c r="F121" t="n">
         <v>-65</v>
@@ -3531,7 +3531,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>7228124300051</t>
+          <t>7228979800010</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
@@ -3540,10 +3540,10 @@
         </is>
       </c>
       <c r="D122" t="n">
-        <v>-64</v>
+        <v>-44</v>
       </c>
       <c r="E122" t="n">
-        <v>-60</v>
+        <v>-48</v>
       </c>
       <c r="F122" t="n">
         <v>-65</v>
@@ -3555,7 +3555,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>7228124300053</t>
+          <t>7228124300045</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -3564,10 +3564,10 @@
         </is>
       </c>
       <c r="D123" t="n">
-        <v>-52</v>
+        <v>-61</v>
       </c>
       <c r="E123" t="n">
-        <v>-62</v>
+        <v>-63</v>
       </c>
       <c r="F123" t="n">
         <v>-65</v>
@@ -3579,7 +3579,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>7228124300054</t>
+          <t>7228124300038</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -3588,10 +3588,10 @@
         </is>
       </c>
       <c r="D124" t="n">
-        <v>-47</v>
+        <v>-54</v>
       </c>
       <c r="E124" t="n">
-        <v>-52</v>
+        <v>-55</v>
       </c>
       <c r="F124" t="n">
         <v>-65</v>
@@ -3603,7 +3603,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>7228124300055</t>
+          <t>7228124200047</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
@@ -3612,10 +3612,10 @@
         </is>
       </c>
       <c r="D125" t="n">
-        <v>-43</v>
+        <v>-50</v>
       </c>
       <c r="E125" t="n">
-        <v>-43</v>
+        <v>-47</v>
       </c>
       <c r="F125" t="n">
         <v>-65</v>
@@ -3627,7 +3627,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>7228124300056</t>
+          <t>7228124200013</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -3636,10 +3636,10 @@
         </is>
       </c>
       <c r="D126" t="n">
-        <v>-57</v>
+        <v>-43</v>
       </c>
       <c r="E126" t="n">
-        <v>-55</v>
+        <v>-49</v>
       </c>
       <c r="F126" t="n">
         <v>-65</v>
@@ -3651,7 +3651,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>7228124300057</t>
+          <t>7228124200022</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
@@ -3660,10 +3660,10 @@
         </is>
       </c>
       <c r="D127" t="n">
-        <v>-41</v>
+        <v>-57</v>
       </c>
       <c r="E127" t="n">
-        <v>-43</v>
+        <v>-50</v>
       </c>
       <c r="F127" t="n">
         <v>-65</v>
@@ -3675,7 +3675,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>7228124300058</t>
+          <t>7228124300047</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
@@ -3684,10 +3684,10 @@
         </is>
       </c>
       <c r="D128" t="n">
-        <v>-57</v>
+        <v>-55</v>
       </c>
       <c r="E128" t="n">
-        <v>-60</v>
+        <v>-51</v>
       </c>
       <c r="F128" t="n">
         <v>-65</v>
@@ -3699,7 +3699,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>7228124300059</t>
+          <t>7228124300014</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
@@ -3708,10 +3708,10 @@
         </is>
       </c>
       <c r="D129" t="n">
-        <v>-50</v>
+        <v>-64</v>
       </c>
       <c r="E129" t="n">
-        <v>-54</v>
+        <v>-63</v>
       </c>
       <c r="F129" t="n">
         <v>-65</v>
@@ -3723,7 +3723,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>7228124300060</t>
+          <t>7228124300018</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
@@ -3732,10 +3732,10 @@
         </is>
       </c>
       <c r="D130" t="n">
-        <v>-62</v>
+        <v>-64</v>
       </c>
       <c r="E130" t="n">
-        <v>-61</v>
+        <v>-63</v>
       </c>
       <c r="F130" t="n">
         <v>-65</v>
@@ -3747,7 +3747,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>7228124300061</t>
+          <t>7228124200069</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
@@ -3756,7 +3756,7 @@
         </is>
       </c>
       <c r="D131" t="n">
-        <v>-53</v>
+        <v>-54</v>
       </c>
       <c r="E131" t="n">
         <v>-55</v>
@@ -3771,7 +3771,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>7228124300062</t>
+          <t>7228124300065</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
@@ -3780,10 +3780,10 @@
         </is>
       </c>
       <c r="D132" t="n">
-        <v>-54</v>
+        <v>-56</v>
       </c>
       <c r="E132" t="n">
-        <v>-49</v>
+        <v>-59</v>
       </c>
       <c r="F132" t="n">
         <v>-65</v>
@@ -3795,7 +3795,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>7228124300063</t>
+          <t>7228124200007</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
@@ -3804,10 +3804,10 @@
         </is>
       </c>
       <c r="D133" t="n">
-        <v>-48</v>
+        <v>-59</v>
       </c>
       <c r="E133" t="n">
-        <v>-55</v>
+        <v>-58</v>
       </c>
       <c r="F133" t="n">
         <v>-65</v>
@@ -3819,7 +3819,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>7228124300065</t>
+          <t>7228124200045</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
@@ -3828,10 +3828,10 @@
         </is>
       </c>
       <c r="D134" t="n">
-        <v>-56</v>
+        <v>-40</v>
       </c>
       <c r="E134" t="n">
-        <v>-59</v>
+        <v>-53</v>
       </c>
       <c r="F134" t="n">
         <v>-65</v>
@@ -3843,7 +3843,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>7228124300066</t>
+          <t>7228124200024</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -3855,7 +3855,7 @@
         <v>-59</v>
       </c>
       <c r="E135" t="n">
-        <v>-61</v>
+        <v>-55</v>
       </c>
       <c r="F135" t="n">
         <v>-65</v>
@@ -3867,7 +3867,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>7228124300067</t>
+          <t>7228124200034</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
@@ -3876,10 +3876,10 @@
         </is>
       </c>
       <c r="D136" t="n">
-        <v>-59</v>
+        <v>-60</v>
       </c>
       <c r="E136" t="n">
-        <v>-58</v>
+        <v>-63</v>
       </c>
       <c r="F136" t="n">
         <v>-65</v>
@@ -3891,7 +3891,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>7228124300068</t>
+          <t>7228124200053</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
@@ -3900,10 +3900,10 @@
         </is>
       </c>
       <c r="D137" t="n">
-        <v>-60</v>
+        <v>-58</v>
       </c>
       <c r="E137" t="n">
-        <v>-64</v>
+        <v>-61</v>
       </c>
       <c r="F137" t="n">
         <v>-65</v>
@@ -3915,7 +3915,7 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>7228124300069</t>
+          <t>7228124300040</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
@@ -3924,10 +3924,10 @@
         </is>
       </c>
       <c r="D138" t="n">
-        <v>-54</v>
+        <v>-62</v>
       </c>
       <c r="E138" t="n">
-        <v>-59</v>
+        <v>-64</v>
       </c>
       <c r="F138" t="n">
         <v>-65</v>
@@ -3939,7 +3939,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>7228124300073</t>
+          <t>7228124300042</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
@@ -3948,10 +3948,10 @@
         </is>
       </c>
       <c r="D139" t="n">
-        <v>-55</v>
+        <v>-58</v>
       </c>
       <c r="E139" t="n">
-        <v>-54</v>
+        <v>-61</v>
       </c>
       <c r="F139" t="n">
         <v>-65</v>
@@ -3963,7 +3963,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>7228124300074</t>
+          <t>7228124200027</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
@@ -3972,10 +3972,10 @@
         </is>
       </c>
       <c r="D140" t="n">
-        <v>-52</v>
+        <v>-65</v>
       </c>
       <c r="E140" t="n">
-        <v>-57</v>
+        <v>-59</v>
       </c>
       <c r="F140" t="n">
         <v>-65</v>
@@ -3987,7 +3987,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>7228124300076</t>
+          <t>7228124200064</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
@@ -4011,7 +4011,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>7228124300077</t>
+          <t>7228124300051</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
@@ -4020,10 +4020,10 @@
         </is>
       </c>
       <c r="D142" t="n">
-        <v>-54</v>
+        <v>-64</v>
       </c>
       <c r="E142" t="n">
-        <v>-52</v>
+        <v>-60</v>
       </c>
       <c r="F142" t="n">
         <v>-65</v>
@@ -4035,7 +4035,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>7228124300078</t>
+          <t>7228124300066</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
@@ -4044,10 +4044,10 @@
         </is>
       </c>
       <c r="D143" t="n">
-        <v>-49</v>
+        <v>-59</v>
       </c>
       <c r="E143" t="n">
-        <v>-50</v>
+        <v>-61</v>
       </c>
       <c r="F143" t="n">
         <v>-65</v>
@@ -4059,7 +4059,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>7228124300081</t>
+          <t>7228124200071</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
@@ -4068,10 +4068,10 @@
         </is>
       </c>
       <c r="D144" t="n">
-        <v>-59</v>
+        <v>-51</v>
       </c>
       <c r="E144" t="n">
-        <v>-60</v>
+        <v>-53</v>
       </c>
       <c r="F144" t="n">
         <v>-65</v>
@@ -4083,7 +4083,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>7228124300082</t>
+          <t>7228124200055</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
@@ -4092,10 +4092,10 @@
         </is>
       </c>
       <c r="D145" t="n">
-        <v>-54</v>
+        <v>-60</v>
       </c>
       <c r="E145" t="n">
-        <v>-51</v>
+        <v>-59</v>
       </c>
       <c r="F145" t="n">
         <v>-65</v>
@@ -4107,7 +4107,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>7228124300083</t>
+          <t>7228124200030</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
@@ -4116,10 +4116,10 @@
         </is>
       </c>
       <c r="D146" t="n">
-        <v>-62</v>
+        <v>-58</v>
       </c>
       <c r="E146" t="n">
-        <v>-59</v>
+        <v>-61</v>
       </c>
       <c r="F146" t="n">
         <v>-65</v>
@@ -4131,7 +4131,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>7228124300084</t>
+          <t>7228124300048</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
@@ -4143,7 +4143,7 @@
         <v>-57</v>
       </c>
       <c r="E147" t="n">
-        <v>-62</v>
+        <v>-59</v>
       </c>
       <c r="F147" t="n">
         <v>-65</v>
@@ -4155,7 +4155,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>7228124300086</t>
+          <t>7228124300049</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
@@ -4164,10 +4164,10 @@
         </is>
       </c>
       <c r="D148" t="n">
-        <v>-50</v>
+        <v>-57</v>
       </c>
       <c r="E148" t="n">
-        <v>-55</v>
+        <v>-62</v>
       </c>
       <c r="F148" t="n">
         <v>-65</v>
@@ -4179,7 +4179,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>7228125100001</t>
+          <t>7228124300055</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
@@ -4188,10 +4188,10 @@
         </is>
       </c>
       <c r="D149" t="n">
-        <v>-56</v>
+        <v>-43</v>
       </c>
       <c r="E149" t="n">
-        <v>-59</v>
+        <v>-43</v>
       </c>
       <c r="F149" t="n">
         <v>-65</v>
@@ -4203,7 +4203,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>7228979800008</t>
+          <t>7228124300078</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
@@ -4212,10 +4212,10 @@
         </is>
       </c>
       <c r="D150" t="n">
-        <v>-55</v>
+        <v>-49</v>
       </c>
       <c r="E150" t="n">
-        <v>-51</v>
+        <v>-50</v>
       </c>
       <c r="F150" t="n">
         <v>-65</v>
@@ -4227,7 +4227,7 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>7228979800009</t>
+          <t>7228124300083</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
@@ -4236,10 +4236,10 @@
         </is>
       </c>
       <c r="D151" t="n">
-        <v>-56</v>
+        <v>-62</v>
       </c>
       <c r="E151" t="n">
-        <v>-52</v>
+        <v>-59</v>
       </c>
       <c r="F151" t="n">
         <v>-65</v>
@@ -4251,7 +4251,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>7228979800010</t>
+          <t>7228124200017</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
@@ -4260,17 +4260,17 @@
         </is>
       </c>
       <c r="D152" t="n">
-        <v>-44</v>
+        <v>-59</v>
       </c>
       <c r="E152" t="n">
-        <v>-48</v>
+        <v>-57</v>
       </c>
       <c r="F152" t="n">
         <v>-65</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new target file to parse
</commit_message>
<xml_diff>
--- a/Auto_RRSIandWiFiSAR_Report/output/WillyWJ_Chen/RSSI.xlsx
+++ b/Auto_RRSIandWiFiSAR_Report/output/WillyWJ_Chen/RSSI.xlsx
@@ -181,7 +181,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'RSSI'!$D$2:$D$144</f>
+              <f>'RSSI'!$D$2:$D$152</f>
             </numRef>
           </val>
         </ser>
@@ -211,7 +211,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'RSSI'!$E$2:$E$144</f>
+              <f>'RSSI'!$E$2:$E$152</f>
             </numRef>
           </val>
         </ser>
@@ -241,7 +241,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'RSSI'!$F$2:$F$144</f>
+              <f>'RSSI'!$F$2:$F$152</f>
             </numRef>
           </val>
         </ser>
@@ -597,7 +597,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F144"/>
+  <dimension ref="A1:F152"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -608,9 +608,9 @@
     <col width="7" customWidth="1" min="1" max="1"/>
     <col width="16" customWidth="1" min="2" max="2"/>
     <col width="14" customWidth="1" min="3" max="3"/>
-    <col width="8" customWidth="1" min="4" max="4"/>
-    <col width="8" customWidth="1" min="5" max="5"/>
-    <col width="8" customWidth="1" min="6" max="6"/>
+    <col width="7" customWidth="1" min="4" max="4"/>
+    <col width="6" customWidth="1" min="5" max="5"/>
+    <col width="7" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -651,7 +651,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>7242218100015</t>
+          <t>7228124300036</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -660,7 +660,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>-47</v>
+        <v>-46</v>
       </c>
       <c r="E2" t="n">
         <v>-48</v>
@@ -675,7 +675,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>7242218100012</t>
+          <t>7228124300026</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -684,10 +684,10 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>-64</v>
+        <v>-61</v>
       </c>
       <c r="E3" t="n">
-        <v>-65</v>
+        <v>-58</v>
       </c>
       <c r="F3" t="n">
         <v>-65</v>
@@ -699,7 +699,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>7242218200038</t>
+          <t>7228124200065</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -708,10 +708,10 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>-61</v>
+        <v>-47</v>
       </c>
       <c r="E4" t="n">
-        <v>-62</v>
+        <v>-54</v>
       </c>
       <c r="F4" t="n">
         <v>-65</v>
@@ -723,7 +723,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>7242213400072</t>
+          <t>7228979800008</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -732,10 +732,10 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>-56</v>
+        <v>-55</v>
       </c>
       <c r="E5" t="n">
-        <v>-52</v>
+        <v>-51</v>
       </c>
       <c r="F5" t="n">
         <v>-65</v>
@@ -747,7 +747,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>7242213400015</t>
+          <t>7228124200054</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -756,10 +756,10 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>-52</v>
+        <v>-47</v>
       </c>
       <c r="E6" t="n">
-        <v>-55</v>
+        <v>-45</v>
       </c>
       <c r="F6" t="n">
         <v>-65</v>
@@ -771,7 +771,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>7242218500005</t>
+          <t>7228124200012</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -780,10 +780,10 @@
         </is>
       </c>
       <c r="D7" t="n">
+        <v>-50</v>
+      </c>
+      <c r="E7" t="n">
         <v>-54</v>
-      </c>
-      <c r="E7" t="n">
-        <v>-56</v>
       </c>
       <c r="F7" t="n">
         <v>-65</v>
@@ -795,7 +795,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>7242218300012</t>
+          <t>7228124300034</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -804,10 +804,10 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>-58</v>
+        <v>-40</v>
       </c>
       <c r="E8" t="n">
-        <v>-53</v>
+        <v>-55</v>
       </c>
       <c r="F8" t="n">
         <v>-65</v>
@@ -819,7 +819,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>7242218200010</t>
+          <t>7228124200036</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -828,10 +828,10 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>-65</v>
+        <v>-53</v>
       </c>
       <c r="E9" t="n">
-        <v>-62</v>
+        <v>-57</v>
       </c>
       <c r="F9" t="n">
         <v>-65</v>
@@ -843,22 +843,22 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>7242213700005</t>
+          <t>7228124300076</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v/>
+        <v>-56</v>
       </c>
       <c r="E10" t="n">
-        <v/>
+        <v>-54</v>
       </c>
       <c r="F10" t="n">
-        <v/>
+        <v>-65</v>
       </c>
     </row>
     <row r="11">
@@ -867,7 +867,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>7242257600007</t>
+          <t>7228124300006</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -876,10 +876,10 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>-43</v>
+        <v>-51</v>
       </c>
       <c r="E11" t="n">
-        <v>-40</v>
+        <v>-56</v>
       </c>
       <c r="F11" t="n">
         <v>-65</v>
@@ -891,7 +891,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>7242213400040</t>
+          <t>7228124200006</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -903,7 +903,7 @@
         <v>-60</v>
       </c>
       <c r="E12" t="n">
-        <v>-53</v>
+        <v>-65</v>
       </c>
       <c r="F12" t="n">
         <v>-65</v>
@@ -915,7 +915,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>7242218300037</t>
+          <t>7228124300012</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -924,10 +924,10 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>-42</v>
+        <v>-53</v>
       </c>
       <c r="E13" t="n">
-        <v>-39</v>
+        <v>-50</v>
       </c>
       <c r="F13" t="n">
         <v>-65</v>
@@ -939,7 +939,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>7242218200026</t>
+          <t>7228124200010</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -948,10 +948,10 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>-55</v>
+        <v>-47</v>
       </c>
       <c r="E14" t="n">
-        <v>-64</v>
+        <v>-58</v>
       </c>
       <c r="F14" t="n">
         <v>-65</v>
@@ -963,7 +963,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>7242214000019</t>
+          <t>7228124200029</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -972,10 +972,10 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>-55</v>
+        <v>-51</v>
       </c>
       <c r="E15" t="n">
-        <v>-49</v>
+        <v>-40</v>
       </c>
       <c r="F15" t="n">
         <v>-65</v>
@@ -987,7 +987,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>7242218200032</t>
+          <t>7228124200025</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -996,10 +996,10 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>-48</v>
+        <v>-57</v>
       </c>
       <c r="E16" t="n">
-        <v>-39</v>
+        <v>-63</v>
       </c>
       <c r="F16" t="n">
         <v>-65</v>
@@ -1011,7 +1011,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>7242214000003</t>
+          <t>7228124300010</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1020,10 +1020,10 @@
         </is>
       </c>
       <c r="D17" t="n">
+        <v>-47</v>
+      </c>
+      <c r="E17" t="n">
         <v>-55</v>
-      </c>
-      <c r="E17" t="n">
-        <v>-48</v>
       </c>
       <c r="F17" t="n">
         <v>-65</v>
@@ -1035,7 +1035,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>7242213400009</t>
+          <t>7228124300077</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1044,10 +1044,10 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>-62</v>
+        <v>-54</v>
       </c>
       <c r="E18" t="n">
-        <v>-60</v>
+        <v>-52</v>
       </c>
       <c r="F18" t="n">
         <v>-65</v>
@@ -1059,7 +1059,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>7242218100006</t>
+          <t>7228124300074</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1068,10 +1068,10 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>-42</v>
+        <v>-52</v>
       </c>
       <c r="E19" t="n">
-        <v>-45</v>
+        <v>-57</v>
       </c>
       <c r="F19" t="n">
         <v>-65</v>
@@ -1083,7 +1083,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>7242218100034</t>
+          <t>7228124300081</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1092,10 +1092,10 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>-54</v>
+        <v>-59</v>
       </c>
       <c r="E20" t="n">
-        <v>-51</v>
+        <v>-60</v>
       </c>
       <c r="F20" t="n">
         <v>-65</v>
@@ -1107,7 +1107,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>7242213400028</t>
+          <t>7228124200033</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1116,10 +1116,10 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>-51</v>
+        <v>-40</v>
       </c>
       <c r="E21" t="n">
-        <v>-49</v>
+        <v>-41</v>
       </c>
       <c r="F21" t="n">
         <v>-65</v>
@@ -1131,7 +1131,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>7242218300035</t>
+          <t>7228124300050</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1140,10 +1140,10 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>-50</v>
+        <v>-56</v>
       </c>
       <c r="E22" t="n">
-        <v>-56</v>
+        <v>-63</v>
       </c>
       <c r="F22" t="n">
         <v>-65</v>
@@ -1155,7 +1155,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>7242218200002</t>
+          <t>7228124300067</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1164,10 +1164,10 @@
         </is>
       </c>
       <c r="D23" t="n">
+        <v>-59</v>
+      </c>
+      <c r="E23" t="n">
         <v>-58</v>
-      </c>
-      <c r="E23" t="n">
-        <v>-65</v>
       </c>
       <c r="F23" t="n">
         <v>-65</v>
@@ -1179,7 +1179,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>7242257600003</t>
+          <t>7228124300058</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1188,10 +1188,10 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>-53</v>
+        <v>-57</v>
       </c>
       <c r="E24" t="n">
-        <v>-52</v>
+        <v>-60</v>
       </c>
       <c r="F24" t="n">
         <v>-65</v>
@@ -1203,7 +1203,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>7242213400047</t>
+          <t>7228125100001</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1212,10 +1212,10 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>-46</v>
+        <v>-56</v>
       </c>
       <c r="E25" t="n">
-        <v>-48</v>
+        <v>-59</v>
       </c>
       <c r="F25" t="n">
         <v>-65</v>
@@ -1227,7 +1227,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>7242214000008</t>
+          <t>7228124300011</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1236,10 +1236,10 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>-54</v>
+        <v>-44</v>
       </c>
       <c r="E26" t="n">
-        <v>-51</v>
+        <v>-41</v>
       </c>
       <c r="F26" t="n">
         <v>-65</v>
@@ -1251,7 +1251,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>7242214000034</t>
+          <t>7228124200043</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1260,10 +1260,10 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>-65</v>
+        <v>-59</v>
       </c>
       <c r="E27" t="n">
-        <v>-65</v>
+        <v>-64</v>
       </c>
       <c r="F27" t="n">
         <v>-65</v>
@@ -1275,7 +1275,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>7242257600004</t>
+          <t>7228124200008</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1284,10 +1284,10 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>-58</v>
+        <v>-63</v>
       </c>
       <c r="E28" t="n">
-        <v>-56</v>
+        <v>-62</v>
       </c>
       <c r="F28" t="n">
         <v>-65</v>
@@ -1299,7 +1299,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>7242218100016</t>
+          <t>7228124200003</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1308,10 +1308,10 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>-53</v>
+        <v>-50</v>
       </c>
       <c r="E29" t="n">
-        <v>-52</v>
+        <v>-46</v>
       </c>
       <c r="F29" t="n">
         <v>-65</v>
@@ -1323,7 +1323,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>7242218300038</t>
+          <t>7228124200060</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1335,7 +1335,7 @@
         <v>-57</v>
       </c>
       <c r="E30" t="n">
-        <v>-58</v>
+        <v>-56</v>
       </c>
       <c r="F30" t="n">
         <v>-65</v>
@@ -1347,7 +1347,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>7242218200017</t>
+          <t>7228101900001</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1356,10 +1356,10 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>-44</v>
+        <v>-50</v>
       </c>
       <c r="E31" t="n">
-        <v>-38</v>
+        <v>-59</v>
       </c>
       <c r="F31" t="n">
         <v>-65</v>
@@ -1371,7 +1371,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>7242218100045</t>
+          <t>7228124200059</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1380,10 +1380,10 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>-43</v>
+        <v>-50</v>
       </c>
       <c r="E32" t="n">
-        <v>-60</v>
+        <v>-56</v>
       </c>
       <c r="F32" t="n">
         <v>-65</v>
@@ -1395,7 +1395,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>7242257600020</t>
+          <t>7228124200028</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1404,10 +1404,10 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>-57</v>
+        <v>-56</v>
       </c>
       <c r="E33" t="n">
-        <v>-64</v>
+        <v>-62</v>
       </c>
       <c r="F33" t="n">
         <v>-65</v>
@@ -1419,7 +1419,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>7242214000016</t>
+          <t>7228124200038</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1428,10 +1428,10 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>-49</v>
+        <v>-57</v>
       </c>
       <c r="E34" t="n">
-        <v>-52</v>
+        <v>-59</v>
       </c>
       <c r="F34" t="n">
         <v>-65</v>
@@ -1443,7 +1443,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>7242218200003</t>
+          <t>7228124300009</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1452,10 +1452,10 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>-54</v>
+        <v>-64</v>
       </c>
       <c r="E35" t="n">
-        <v>-45</v>
+        <v>-64</v>
       </c>
       <c r="F35" t="n">
         <v>-65</v>
@@ -1467,7 +1467,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>7242218100001</t>
+          <t>7228124300053</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1479,7 +1479,7 @@
         <v>-52</v>
       </c>
       <c r="E36" t="n">
-        <v>-56</v>
+        <v>-62</v>
       </c>
       <c r="F36" t="n">
         <v>-65</v>
@@ -1491,7 +1491,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>7242218100005</t>
+          <t>7228124300084</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1500,10 +1500,10 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>-52</v>
+        <v>-57</v>
       </c>
       <c r="E37" t="n">
-        <v>-54</v>
+        <v>-62</v>
       </c>
       <c r="F37" t="n">
         <v>-65</v>
@@ -1515,7 +1515,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>7242218400002</t>
+          <t>7228124200039</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1524,10 +1524,10 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>-58</v>
+        <v>-56</v>
       </c>
       <c r="E38" t="n">
-        <v>-60</v>
+        <v>-65</v>
       </c>
       <c r="F38" t="n">
         <v>-65</v>
@@ -1539,7 +1539,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>7242213400016</t>
+          <t>7228124200018</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1548,10 +1548,10 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>-41</v>
+        <v>-59</v>
       </c>
       <c r="E39" t="n">
-        <v>-44</v>
+        <v>-60</v>
       </c>
       <c r="F39" t="n">
         <v>-65</v>
@@ -1563,7 +1563,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>7242213400039</t>
+          <t>7228124200002</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1572,10 +1572,10 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>-57</v>
+        <v>-61</v>
       </c>
       <c r="E40" t="n">
-        <v>-56</v>
+        <v>-65</v>
       </c>
       <c r="F40" t="n">
         <v>-65</v>
@@ -1587,7 +1587,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>7242218200015</t>
+          <t>7228124200019</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1596,10 +1596,10 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>-57</v>
+        <v>-53</v>
       </c>
       <c r="E41" t="n">
-        <v>-56</v>
+        <v>-50</v>
       </c>
       <c r="F41" t="n">
         <v>-65</v>
@@ -1611,7 +1611,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>7242213500034</t>
+          <t>7228124200067</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1620,10 +1620,10 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>-49</v>
+        <v>-61</v>
       </c>
       <c r="E42" t="n">
-        <v>-53</v>
+        <v>-61</v>
       </c>
       <c r="F42" t="n">
         <v>-65</v>
@@ -1635,7 +1635,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>7242218200007</t>
+          <t>7228124300069</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1644,10 +1644,10 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>-49</v>
+        <v>-54</v>
       </c>
       <c r="E43" t="n">
-        <v>-50</v>
+        <v>-59</v>
       </c>
       <c r="F43" t="n">
         <v>-65</v>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>7242218100003</t>
+          <t>7228124200004</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1668,10 +1668,10 @@
         </is>
       </c>
       <c r="D44" t="n">
+        <v>-49</v>
+      </c>
+      <c r="E44" t="n">
         <v>-55</v>
-      </c>
-      <c r="E44" t="n">
-        <v>-52</v>
       </c>
       <c r="F44" t="n">
         <v>-65</v>
@@ -1683,7 +1683,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>7242213400033</t>
+          <t>7228124300033</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1692,10 +1692,10 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>-51</v>
+        <v>-60</v>
       </c>
       <c r="E45" t="n">
-        <v>-49</v>
+        <v>-60</v>
       </c>
       <c r="F45" t="n">
         <v>-65</v>
@@ -1707,7 +1707,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>7242213400006</t>
+          <t>7228124300035</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1716,10 +1716,10 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>-55</v>
+        <v>-45</v>
       </c>
       <c r="E46" t="n">
-        <v>-51</v>
+        <v>-57</v>
       </c>
       <c r="F46" t="n">
         <v>-65</v>
@@ -1731,7 +1731,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>7242257600015</t>
+          <t>7228124300016</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1740,10 +1740,10 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>-53</v>
+        <v>-60</v>
       </c>
       <c r="E47" t="n">
-        <v>-52</v>
+        <v>-62</v>
       </c>
       <c r="F47" t="n">
         <v>-65</v>
@@ -1755,7 +1755,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>7242257600018</t>
+          <t>7228124200040</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1764,10 +1764,10 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>-49</v>
+        <v>-62</v>
       </c>
       <c r="E48" t="n">
-        <v>-47</v>
+        <v>-64</v>
       </c>
       <c r="F48" t="n">
         <v>-65</v>
@@ -1779,7 +1779,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>7242218300021</t>
+          <t>7224908800005</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1788,10 +1788,10 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>-44</v>
+        <v>-61</v>
       </c>
       <c r="E49" t="n">
-        <v>-42</v>
+        <v>-62</v>
       </c>
       <c r="F49" t="n">
         <v>-65</v>
@@ -1803,7 +1803,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>7242218200035</t>
+          <t>7228124200042</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1812,10 +1812,10 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>-46</v>
+        <v>-60</v>
       </c>
       <c r="E50" t="n">
-        <v>-39</v>
+        <v>-60</v>
       </c>
       <c r="F50" t="n">
         <v>-65</v>
@@ -1827,7 +1827,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>7242218200039</t>
+          <t>7228124300028</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1836,10 +1836,10 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>-56</v>
+        <v>-65</v>
       </c>
       <c r="E51" t="n">
-        <v>-57</v>
+        <v>-61</v>
       </c>
       <c r="F51" t="n">
         <v>-65</v>
@@ -1851,7 +1851,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>7242218100026</t>
+          <t>7228124200052</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1860,10 +1860,10 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>-49</v>
+        <v>-64</v>
       </c>
       <c r="E52" t="n">
-        <v>-48</v>
+        <v>-58</v>
       </c>
       <c r="F52" t="n">
         <v>-65</v>
@@ -1875,7 +1875,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>7242218100035</t>
+          <t>7228124300057</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1884,10 +1884,10 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>-45</v>
+        <v>-41</v>
       </c>
       <c r="E53" t="n">
-        <v>-45</v>
+        <v>-43</v>
       </c>
       <c r="F53" t="n">
         <v>-65</v>
@@ -1899,22 +1899,22 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>7242213600048</t>
+          <t>7228124200051</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v/>
+        <v>-64</v>
       </c>
       <c r="E54" t="n">
-        <v/>
+        <v>-64</v>
       </c>
       <c r="F54" t="n">
-        <v/>
+        <v>-65</v>
       </c>
     </row>
     <row r="55">
@@ -1923,7 +1923,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>7242218300010</t>
+          <t>7228124200037</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -1932,10 +1932,10 @@
         </is>
       </c>
       <c r="D55" t="n">
-        <v>-61</v>
+        <v>-41</v>
       </c>
       <c r="E55" t="n">
-        <v>-60</v>
+        <v>-59</v>
       </c>
       <c r="F55" t="n">
         <v>-65</v>
@@ -1947,7 +1947,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>7242218300022</t>
+          <t>7228124200076</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -1956,10 +1956,10 @@
         </is>
       </c>
       <c r="D56" t="n">
-        <v>-54</v>
+        <v>-62</v>
       </c>
       <c r="E56" t="n">
-        <v>-55</v>
+        <v>-64</v>
       </c>
       <c r="F56" t="n">
         <v>-65</v>
@@ -1971,7 +1971,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>7242218100010</t>
+          <t>7228124200084</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -1980,10 +1980,10 @@
         </is>
       </c>
       <c r="D57" t="n">
-        <v>-63</v>
+        <v>-38</v>
       </c>
       <c r="E57" t="n">
-        <v>-63</v>
+        <v>-48</v>
       </c>
       <c r="F57" t="n">
         <v>-65</v>
@@ -1995,7 +1995,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>7242218200014</t>
+          <t>7228101600001</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2004,10 +2004,10 @@
         </is>
       </c>
       <c r="D58" t="n">
-        <v>-46</v>
+        <v>-60</v>
       </c>
       <c r="E58" t="n">
-        <v>-55</v>
+        <v>-54</v>
       </c>
       <c r="F58" t="n">
         <v>-65</v>
@@ -2019,7 +2019,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>7242213500020</t>
+          <t>7228124300032</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -2028,10 +2028,10 @@
         </is>
       </c>
       <c r="D59" t="n">
-        <v>-57</v>
+        <v>-53</v>
       </c>
       <c r="E59" t="n">
-        <v>-55</v>
+        <v>-52</v>
       </c>
       <c r="F59" t="n">
         <v>-65</v>
@@ -2043,7 +2043,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>7242218200016</t>
+          <t>7228124200005</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2052,10 +2052,10 @@
         </is>
       </c>
       <c r="D60" t="n">
-        <v>-53</v>
+        <v>-58</v>
       </c>
       <c r="E60" t="n">
-        <v>-51</v>
+        <v>-58</v>
       </c>
       <c r="F60" t="n">
         <v>-65</v>
@@ -2067,7 +2067,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>7242213500016</t>
+          <t>7228124200062</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2076,10 +2076,10 @@
         </is>
       </c>
       <c r="D61" t="n">
-        <v>-60</v>
+        <v>-53</v>
       </c>
       <c r="E61" t="n">
-        <v>-64</v>
+        <v>-53</v>
       </c>
       <c r="F61" t="n">
         <v>-65</v>
@@ -2091,7 +2091,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>7242218200028</t>
+          <t>7228124200014</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2100,10 +2100,10 @@
         </is>
       </c>
       <c r="D62" t="n">
-        <v>-42</v>
+        <v>-49</v>
       </c>
       <c r="E62" t="n">
-        <v>-43</v>
+        <v>-48</v>
       </c>
       <c r="F62" t="n">
         <v>-65</v>
@@ -2115,7 +2115,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>7242213400076</t>
+          <t>7228124200080</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -2124,10 +2124,10 @@
         </is>
       </c>
       <c r="D63" t="n">
-        <v>-53</v>
+        <v>-60</v>
       </c>
       <c r="E63" t="n">
-        <v>-57</v>
+        <v>-62</v>
       </c>
       <c r="F63" t="n">
         <v>-65</v>
@@ -2139,7 +2139,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>7242214000010</t>
+          <t>7228124200057</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -2148,10 +2148,10 @@
         </is>
       </c>
       <c r="D64" t="n">
+        <v>-55</v>
+      </c>
+      <c r="E64" t="n">
         <v>-57</v>
-      </c>
-      <c r="E64" t="n">
-        <v>-60</v>
       </c>
       <c r="F64" t="n">
         <v>-65</v>
@@ -2163,7 +2163,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>7242257600009</t>
+          <t>7228124300063</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -2172,10 +2172,10 @@
         </is>
       </c>
       <c r="D65" t="n">
+        <v>-48</v>
+      </c>
+      <c r="E65" t="n">
         <v>-55</v>
-      </c>
-      <c r="E65" t="n">
-        <v>-58</v>
       </c>
       <c r="F65" t="n">
         <v>-65</v>
@@ -2187,7 +2187,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>7242214000025</t>
+          <t>7228124200077</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2196,10 +2196,10 @@
         </is>
       </c>
       <c r="D66" t="n">
-        <v>-47</v>
+        <v>-61</v>
       </c>
       <c r="E66" t="n">
-        <v>-51</v>
+        <v>-57</v>
       </c>
       <c r="F66" t="n">
         <v>-65</v>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>7242218400006</t>
+          <t>7228124200048</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2220,10 +2220,10 @@
         </is>
       </c>
       <c r="D67" t="n">
-        <v>-50</v>
+        <v>-49</v>
       </c>
       <c r="E67" t="n">
-        <v>-50</v>
+        <v>-52</v>
       </c>
       <c r="F67" t="n">
         <v>-65</v>
@@ -2235,7 +2235,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>7242218100013</t>
+          <t>7228124300030</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -2244,10 +2244,10 @@
         </is>
       </c>
       <c r="D68" t="n">
-        <v>-64</v>
+        <v>-48</v>
       </c>
       <c r="E68" t="n">
-        <v>-65</v>
+        <v>-51</v>
       </c>
       <c r="F68" t="n">
         <v>-65</v>
@@ -2259,7 +2259,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>7242218400004</t>
+          <t>7228124300062</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -2268,10 +2268,10 @@
         </is>
       </c>
       <c r="D69" t="n">
-        <v>-51</v>
+        <v>-54</v>
       </c>
       <c r="E69" t="n">
-        <v>-51</v>
+        <v>-49</v>
       </c>
       <c r="F69" t="n">
         <v>-65</v>
@@ -2283,7 +2283,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>7242257600014</t>
+          <t>7228101300001</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -2292,10 +2292,10 @@
         </is>
       </c>
       <c r="D70" t="n">
-        <v>-54</v>
+        <v>-60</v>
       </c>
       <c r="E70" t="n">
-        <v>-56</v>
+        <v>-63</v>
       </c>
       <c r="F70" t="n">
         <v>-65</v>
@@ -2307,7 +2307,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>7242213400062</t>
+          <t>7228124200066</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -2316,10 +2316,10 @@
         </is>
       </c>
       <c r="D71" t="n">
+        <v>-59</v>
+      </c>
+      <c r="E71" t="n">
         <v>-56</v>
-      </c>
-      <c r="E71" t="n">
-        <v>-52</v>
       </c>
       <c r="F71" t="n">
         <v>-65</v>
@@ -2331,7 +2331,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>7242218100037</t>
+          <t>7228124200082</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -2340,10 +2340,10 @@
         </is>
       </c>
       <c r="D72" t="n">
-        <v>-52</v>
+        <v>-63</v>
       </c>
       <c r="E72" t="n">
-        <v>-53</v>
+        <v>-63</v>
       </c>
       <c r="F72" t="n">
         <v>-65</v>
@@ -2355,7 +2355,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>7242213400065</t>
+          <t>7228124200020</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -2364,7 +2364,7 @@
         </is>
       </c>
       <c r="D73" t="n">
-        <v>-50</v>
+        <v>-53</v>
       </c>
       <c r="E73" t="n">
         <v>-50</v>
@@ -2379,7 +2379,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>7242213400058</t>
+          <t>7228124200044</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -2388,10 +2388,10 @@
         </is>
       </c>
       <c r="D74" t="n">
-        <v>-51</v>
+        <v>-55</v>
       </c>
       <c r="E74" t="n">
-        <v>-53</v>
+        <v>-46</v>
       </c>
       <c r="F74" t="n">
         <v>-65</v>
@@ -2403,7 +2403,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>7242218200008</t>
+          <t>7228124300024</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -2412,10 +2412,10 @@
         </is>
       </c>
       <c r="D75" t="n">
-        <v>-52</v>
+        <v>-59</v>
       </c>
       <c r="E75" t="n">
-        <v>-55</v>
+        <v>-57</v>
       </c>
       <c r="F75" t="n">
         <v>-65</v>
@@ -2427,7 +2427,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>7242257600001</t>
+          <t>7228124200021</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -2436,10 +2436,10 @@
         </is>
       </c>
       <c r="D76" t="n">
-        <v>-55</v>
+        <v>-65</v>
       </c>
       <c r="E76" t="n">
-        <v>-60</v>
+        <v>-65</v>
       </c>
       <c r="F76" t="n">
         <v>-65</v>
@@ -2451,7 +2451,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>7242213400077</t>
+          <t>7228124200058</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -2460,10 +2460,10 @@
         </is>
       </c>
       <c r="D77" t="n">
-        <v>-59</v>
+        <v>-57</v>
       </c>
       <c r="E77" t="n">
-        <v>-59</v>
+        <v>-62</v>
       </c>
       <c r="F77" t="n">
         <v>-65</v>
@@ -2475,7 +2475,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>7242218300002</t>
+          <t>7224908800006</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -2484,10 +2484,10 @@
         </is>
       </c>
       <c r="D78" t="n">
-        <v>-56</v>
+        <v>-62</v>
       </c>
       <c r="E78" t="n">
-        <v>-59</v>
+        <v>-60</v>
       </c>
       <c r="F78" t="n">
         <v>-65</v>
@@ -2499,7 +2499,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>7242218300030</t>
+          <t>7228124200068</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -2508,10 +2508,10 @@
         </is>
       </c>
       <c r="D79" t="n">
-        <v>-39</v>
+        <v>-56</v>
       </c>
       <c r="E79" t="n">
-        <v>-43</v>
+        <v>-51</v>
       </c>
       <c r="F79" t="n">
         <v>-65</v>
@@ -2523,7 +2523,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>7242218200011</t>
+          <t>7228124300073</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -2532,10 +2532,10 @@
         </is>
       </c>
       <c r="D80" t="n">
-        <v>-47</v>
+        <v>-55</v>
       </c>
       <c r="E80" t="n">
-        <v>-44</v>
+        <v>-54</v>
       </c>
       <c r="F80" t="n">
         <v>-65</v>
@@ -2547,7 +2547,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>7242213500025</t>
+          <t>7228124200078</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -2556,10 +2556,10 @@
         </is>
       </c>
       <c r="D81" t="n">
-        <v>-55</v>
+        <v>-60</v>
       </c>
       <c r="E81" t="n">
-        <v>-49</v>
+        <v>-61</v>
       </c>
       <c r="F81" t="n">
         <v>-65</v>
@@ -2571,7 +2571,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>7242213400067</t>
+          <t>7228101400001</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -2580,10 +2580,10 @@
         </is>
       </c>
       <c r="D82" t="n">
-        <v>-47</v>
+        <v>-55</v>
       </c>
       <c r="E82" t="n">
-        <v>-36</v>
+        <v>-58</v>
       </c>
       <c r="F82" t="n">
         <v>-65</v>
@@ -2595,7 +2595,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>7242213400048</t>
+          <t>7228124200056</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -2604,10 +2604,10 @@
         </is>
       </c>
       <c r="D83" t="n">
-        <v>-49</v>
+        <v>-65</v>
       </c>
       <c r="E83" t="n">
-        <v>-49</v>
+        <v>-62</v>
       </c>
       <c r="F83" t="n">
         <v>-65</v>
@@ -2619,7 +2619,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>7242218200006</t>
+          <t>7228124200070</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -2628,10 +2628,10 @@
         </is>
       </c>
       <c r="D84" t="n">
-        <v>-52</v>
+        <v>-61</v>
       </c>
       <c r="E84" t="n">
-        <v>-46</v>
+        <v>-63</v>
       </c>
       <c r="F84" t="n">
         <v>-65</v>
@@ -2643,7 +2643,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>7242214000026</t>
+          <t>7228124300025</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -2652,10 +2652,10 @@
         </is>
       </c>
       <c r="D85" t="n">
-        <v>-60</v>
+        <v>-54</v>
       </c>
       <c r="E85" t="n">
-        <v>-58</v>
+        <v>-51</v>
       </c>
       <c r="F85" t="n">
         <v>-65</v>
@@ -2667,7 +2667,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>7242218300029</t>
+          <t>7228124300015</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -2676,10 +2676,10 @@
         </is>
       </c>
       <c r="D86" t="n">
-        <v>-43</v>
+        <v>-64</v>
       </c>
       <c r="E86" t="n">
-        <v>-40</v>
+        <v>-61</v>
       </c>
       <c r="F86" t="n">
         <v>-65</v>
@@ -2691,7 +2691,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>7242218100029</t>
+          <t>7228124200085</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -2700,10 +2700,10 @@
         </is>
       </c>
       <c r="D87" t="n">
-        <v>-52</v>
+        <v>-63</v>
       </c>
       <c r="E87" t="n">
-        <v>-58</v>
+        <v>-65</v>
       </c>
       <c r="F87" t="n">
         <v>-65</v>
@@ -2715,7 +2715,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>7242213400054</t>
+          <t>7224908800007</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -2724,10 +2724,10 @@
         </is>
       </c>
       <c r="D88" t="n">
-        <v>-50</v>
+        <v>-60</v>
       </c>
       <c r="E88" t="n">
-        <v>-51</v>
+        <v>-60</v>
       </c>
       <c r="F88" t="n">
         <v>-65</v>
@@ -2739,7 +2739,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>7242218300036</t>
+          <t>7228124300020</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -2748,10 +2748,10 @@
         </is>
       </c>
       <c r="D89" t="n">
-        <v>-54</v>
+        <v>-51</v>
       </c>
       <c r="E89" t="n">
-        <v>-55</v>
+        <v>-57</v>
       </c>
       <c r="F89" t="n">
         <v>-65</v>
@@ -2763,7 +2763,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>7242218400001</t>
+          <t>7228124300019</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -2772,10 +2772,10 @@
         </is>
       </c>
       <c r="D90" t="n">
-        <v>-40</v>
+        <v>-55</v>
       </c>
       <c r="E90" t="n">
-        <v>-43</v>
+        <v>-50</v>
       </c>
       <c r="F90" t="n">
         <v>-65</v>
@@ -2787,7 +2787,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>7242214000006</t>
+          <t>7228124200061</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -2799,7 +2799,7 @@
         <v>-51</v>
       </c>
       <c r="E91" t="n">
-        <v>-52</v>
+        <v>-60</v>
       </c>
       <c r="F91" t="n">
         <v>-65</v>
@@ -2811,7 +2811,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>7242213500023</t>
+          <t>7228124300002</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -2820,10 +2820,10 @@
         </is>
       </c>
       <c r="D92" t="n">
-        <v>-53</v>
+        <v>-43</v>
       </c>
       <c r="E92" t="n">
-        <v>-50</v>
+        <v>-59</v>
       </c>
       <c r="F92" t="n">
         <v>-65</v>
@@ -2835,7 +2835,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>7242213400043</t>
+          <t>7228124200041</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -2844,7 +2844,7 @@
         </is>
       </c>
       <c r="D93" t="n">
-        <v>-50</v>
+        <v>-49</v>
       </c>
       <c r="E93" t="n">
         <v>-53</v>
@@ -2859,7 +2859,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>7242218200023</t>
+          <t>7228124300068</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -2868,10 +2868,10 @@
         </is>
       </c>
       <c r="D94" t="n">
-        <v>-47</v>
+        <v>-60</v>
       </c>
       <c r="E94" t="n">
-        <v>-53</v>
+        <v>-64</v>
       </c>
       <c r="F94" t="n">
         <v>-65</v>
@@ -2883,7 +2883,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>7242257600019</t>
+          <t>7228124300031</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -2892,10 +2892,10 @@
         </is>
       </c>
       <c r="D95" t="n">
-        <v>-54</v>
+        <v>-53</v>
       </c>
       <c r="E95" t="n">
-        <v>-52</v>
+        <v>-58</v>
       </c>
       <c r="F95" t="n">
         <v>-65</v>
@@ -2907,7 +2907,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>7242218100042</t>
+          <t>7228124300013</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -2916,10 +2916,10 @@
         </is>
       </c>
       <c r="D96" t="n">
-        <v>-46</v>
+        <v>-55</v>
       </c>
       <c r="E96" t="n">
-        <v>-49</v>
+        <v>-65</v>
       </c>
       <c r="F96" t="n">
         <v>-65</v>
@@ -2931,7 +2931,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>7242218200030</t>
+          <t>7228124300056</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -2940,10 +2940,10 @@
         </is>
       </c>
       <c r="D97" t="n">
-        <v>-64</v>
+        <v>-57</v>
       </c>
       <c r="E97" t="n">
-        <v>-64</v>
+        <v>-55</v>
       </c>
       <c r="F97" t="n">
         <v>-65</v>
@@ -2955,7 +2955,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>7242218300025</t>
+          <t>7228124200035</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -2964,10 +2964,10 @@
         </is>
       </c>
       <c r="D98" t="n">
-        <v>-51</v>
+        <v>-65</v>
       </c>
       <c r="E98" t="n">
-        <v>-50</v>
+        <v>-60</v>
       </c>
       <c r="F98" t="n">
         <v>-65</v>
@@ -2979,7 +2979,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>7242218100007</t>
+          <t>7228979800009</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -2988,10 +2988,10 @@
         </is>
       </c>
       <c r="D99" t="n">
-        <v>-53</v>
+        <v>-56</v>
       </c>
       <c r="E99" t="n">
-        <v>-50</v>
+        <v>-52</v>
       </c>
       <c r="F99" t="n">
         <v>-65</v>
@@ -3003,7 +3003,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>7242214000017</t>
+          <t>7228124300054</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -3012,10 +3012,10 @@
         </is>
       </c>
       <c r="D100" t="n">
-        <v>-59</v>
+        <v>-47</v>
       </c>
       <c r="E100" t="n">
-        <v>-56</v>
+        <v>-52</v>
       </c>
       <c r="F100" t="n">
         <v>-65</v>
@@ -3027,7 +3027,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>7242218100002</t>
+          <t>7228124200031</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -3036,10 +3036,10 @@
         </is>
       </c>
       <c r="D101" t="n">
-        <v>-54</v>
+        <v>-53</v>
       </c>
       <c r="E101" t="n">
-        <v>-49</v>
+        <v>-50</v>
       </c>
       <c r="F101" t="n">
         <v>-65</v>
@@ -3051,7 +3051,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>7242213500010</t>
+          <t>7228124300041</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -3060,10 +3060,10 @@
         </is>
       </c>
       <c r="D102" t="n">
-        <v>-51</v>
+        <v>-57</v>
       </c>
       <c r="E102" t="n">
-        <v>-49</v>
+        <v>-53</v>
       </c>
       <c r="F102" t="n">
         <v>-65</v>
@@ -3075,7 +3075,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>7242218100019</t>
+          <t>7228124200026</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -3084,10 +3084,10 @@
         </is>
       </c>
       <c r="D103" t="n">
-        <v>-53</v>
+        <v>-55</v>
       </c>
       <c r="E103" t="n">
-        <v>-54</v>
+        <v>-60</v>
       </c>
       <c r="F103" t="n">
         <v>-65</v>
@@ -3099,7 +3099,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>7242218100025</t>
+          <t>7228124300039</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -3108,10 +3108,10 @@
         </is>
       </c>
       <c r="D104" t="n">
-        <v>-45</v>
+        <v>-47</v>
       </c>
       <c r="E104" t="n">
-        <v>-45</v>
+        <v>-53</v>
       </c>
       <c r="F104" t="n">
         <v>-65</v>
@@ -3123,7 +3123,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>7242213500019</t>
+          <t>7228124300037</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -3132,10 +3132,10 @@
         </is>
       </c>
       <c r="D105" t="n">
-        <v>-54</v>
+        <v>-56</v>
       </c>
       <c r="E105" t="n">
-        <v>-57</v>
+        <v>-55</v>
       </c>
       <c r="F105" t="n">
         <v>-65</v>
@@ -3147,7 +3147,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>7242218100033</t>
+          <t>7228124300061</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -3156,10 +3156,10 @@
         </is>
       </c>
       <c r="D106" t="n">
-        <v>-43</v>
+        <v>-53</v>
       </c>
       <c r="E106" t="n">
-        <v>-52</v>
+        <v>-55</v>
       </c>
       <c r="F106" t="n">
         <v>-65</v>
@@ -3171,7 +3171,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>7242213500032</t>
+          <t>7228124200046</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -3180,10 +3180,10 @@
         </is>
       </c>
       <c r="D107" t="n">
-        <v>-47</v>
+        <v>-61</v>
       </c>
       <c r="E107" t="n">
-        <v>-44</v>
+        <v>-65</v>
       </c>
       <c r="F107" t="n">
         <v>-65</v>
@@ -3195,7 +3195,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>7242213500033</t>
+          <t>7228124200075</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -3204,10 +3204,10 @@
         </is>
       </c>
       <c r="D108" t="n">
-        <v>-62</v>
+        <v>-58</v>
       </c>
       <c r="E108" t="n">
-        <v>-65</v>
+        <v>-56</v>
       </c>
       <c r="F108" t="n">
         <v>-65</v>
@@ -3219,7 +3219,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>7242218200012</t>
+          <t>7228124300003</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -3228,10 +3228,10 @@
         </is>
       </c>
       <c r="D109" t="n">
-        <v>-45</v>
+        <v>-57</v>
       </c>
       <c r="E109" t="n">
-        <v>-45</v>
+        <v>-58</v>
       </c>
       <c r="F109" t="n">
         <v>-65</v>
@@ -3243,7 +3243,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>7242218100038</t>
+          <t>7228124300029</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -3252,10 +3252,10 @@
         </is>
       </c>
       <c r="D110" t="n">
-        <v>-30</v>
+        <v>-57</v>
       </c>
       <c r="E110" t="n">
-        <v>-41</v>
+        <v>-65</v>
       </c>
       <c r="F110" t="n">
         <v>-65</v>
@@ -3267,7 +3267,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>7242257600017</t>
+          <t>7228124300082</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -3276,10 +3276,10 @@
         </is>
       </c>
       <c r="D111" t="n">
-        <v>-50</v>
+        <v>-54</v>
       </c>
       <c r="E111" t="n">
-        <v>-47</v>
+        <v>-51</v>
       </c>
       <c r="F111" t="n">
         <v>-65</v>
@@ -3291,7 +3291,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>7242218300024</t>
+          <t>7228124200023</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -3300,10 +3300,10 @@
         </is>
       </c>
       <c r="D112" t="n">
-        <v>-55</v>
+        <v>-54</v>
       </c>
       <c r="E112" t="n">
-        <v>-48</v>
+        <v>-49</v>
       </c>
       <c r="F112" t="n">
         <v>-65</v>
@@ -3315,7 +3315,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>7242218100031</t>
+          <t>7228124300060</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -3324,10 +3324,10 @@
         </is>
       </c>
       <c r="D113" t="n">
-        <v>-49</v>
+        <v>-62</v>
       </c>
       <c r="E113" t="n">
-        <v>-56</v>
+        <v>-61</v>
       </c>
       <c r="F113" t="n">
         <v>-65</v>
@@ -3339,7 +3339,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>7242218200021</t>
+          <t>7228124200049</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -3348,10 +3348,10 @@
         </is>
       </c>
       <c r="D114" t="n">
-        <v>-51</v>
+        <v>-62</v>
       </c>
       <c r="E114" t="n">
-        <v>-54</v>
+        <v>-58</v>
       </c>
       <c r="F114" t="n">
         <v>-65</v>
@@ -3363,7 +3363,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>7242213400052</t>
+          <t>7228101700001</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -3372,10 +3372,10 @@
         </is>
       </c>
       <c r="D115" t="n">
-        <v>-50</v>
+        <v>-53</v>
       </c>
       <c r="E115" t="n">
-        <v>-51</v>
+        <v>-59</v>
       </c>
       <c r="F115" t="n">
         <v>-65</v>
@@ -3387,7 +3387,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>7242213500026</t>
+          <t>7228124300023</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -3396,10 +3396,10 @@
         </is>
       </c>
       <c r="D116" t="n">
-        <v>-49</v>
+        <v>-51</v>
       </c>
       <c r="E116" t="n">
-        <v>-57</v>
+        <v>-51</v>
       </c>
       <c r="F116" t="n">
         <v>-65</v>
@@ -3411,7 +3411,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>7242214000020</t>
+          <t>7228124300086</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -3420,10 +3420,10 @@
         </is>
       </c>
       <c r="D117" t="n">
-        <v>-46</v>
+        <v>-50</v>
       </c>
       <c r="E117" t="n">
-        <v>-47</v>
+        <v>-55</v>
       </c>
       <c r="F117" t="n">
         <v>-65</v>
@@ -3435,7 +3435,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>7242218500004</t>
+          <t>7228124300059</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -3447,7 +3447,7 @@
         <v>-50</v>
       </c>
       <c r="E118" t="n">
-        <v>-50</v>
+        <v>-54</v>
       </c>
       <c r="F118" t="n">
         <v>-65</v>
@@ -3459,7 +3459,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>7242257600016</t>
+          <t>7228124200079</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -3468,10 +3468,10 @@
         </is>
       </c>
       <c r="D119" t="n">
-        <v>-52</v>
+        <v>-64</v>
       </c>
       <c r="E119" t="n">
-        <v>-56</v>
+        <v>-65</v>
       </c>
       <c r="F119" t="n">
         <v>-65</v>
@@ -3483,7 +3483,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>7242218300014</t>
+          <t>7228124100001</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
@@ -3492,10 +3492,10 @@
         </is>
       </c>
       <c r="D120" t="n">
-        <v>-38</v>
+        <v>-54</v>
       </c>
       <c r="E120" t="n">
-        <v>-45</v>
+        <v>-63</v>
       </c>
       <c r="F120" t="n">
         <v>-65</v>
@@ -3507,7 +3507,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>7242218300028</t>
+          <t>7228124200081</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
@@ -3516,10 +3516,10 @@
         </is>
       </c>
       <c r="D121" t="n">
-        <v>-59</v>
+        <v>-49</v>
       </c>
       <c r="E121" t="n">
-        <v>-60</v>
+        <v>-45</v>
       </c>
       <c r="F121" t="n">
         <v>-65</v>
@@ -3531,7 +3531,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>7242218300031</t>
+          <t>7228979800010</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
@@ -3540,10 +3540,10 @@
         </is>
       </c>
       <c r="D122" t="n">
-        <v>-58</v>
+        <v>-44</v>
       </c>
       <c r="E122" t="n">
-        <v>-55</v>
+        <v>-48</v>
       </c>
       <c r="F122" t="n">
         <v>-65</v>
@@ -3555,7 +3555,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>7242214000021</t>
+          <t>7228124300045</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -3564,10 +3564,10 @@
         </is>
       </c>
       <c r="D123" t="n">
-        <v>-37</v>
+        <v>-61</v>
       </c>
       <c r="E123" t="n">
-        <v>-37</v>
+        <v>-63</v>
       </c>
       <c r="F123" t="n">
         <v>-65</v>
@@ -3579,7 +3579,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>7242213400050</t>
+          <t>7228124300038</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -3591,7 +3591,7 @@
         <v>-54</v>
       </c>
       <c r="E124" t="n">
-        <v>-52</v>
+        <v>-55</v>
       </c>
       <c r="F124" t="n">
         <v>-65</v>
@@ -3603,7 +3603,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>7242218200013</t>
+          <t>7228124200047</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
@@ -3612,10 +3612,10 @@
         </is>
       </c>
       <c r="D125" t="n">
-        <v>-44</v>
+        <v>-50</v>
       </c>
       <c r="E125" t="n">
-        <v>-50</v>
+        <v>-47</v>
       </c>
       <c r="F125" t="n">
         <v>-65</v>
@@ -3627,7 +3627,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>7242218300039</t>
+          <t>7228124200013</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -3636,10 +3636,10 @@
         </is>
       </c>
       <c r="D126" t="n">
-        <v>-56</v>
+        <v>-43</v>
       </c>
       <c r="E126" t="n">
-        <v>-48</v>
+        <v>-49</v>
       </c>
       <c r="F126" t="n">
         <v>-65</v>
@@ -3651,7 +3651,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>7242218300027</t>
+          <t>7228124200022</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
@@ -3660,10 +3660,10 @@
         </is>
       </c>
       <c r="D127" t="n">
-        <v>-49</v>
+        <v>-57</v>
       </c>
       <c r="E127" t="n">
-        <v>-46</v>
+        <v>-50</v>
       </c>
       <c r="F127" t="n">
         <v>-65</v>
@@ -3675,7 +3675,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>7242213400014</t>
+          <t>7228124300047</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
@@ -3684,10 +3684,10 @@
         </is>
       </c>
       <c r="D128" t="n">
-        <v>-42</v>
+        <v>-55</v>
       </c>
       <c r="E128" t="n">
-        <v>-41</v>
+        <v>-51</v>
       </c>
       <c r="F128" t="n">
         <v>-65</v>
@@ -3699,7 +3699,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>7242218300015</t>
+          <t>7228124300014</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
@@ -3708,10 +3708,10 @@
         </is>
       </c>
       <c r="D129" t="n">
-        <v>-59</v>
+        <v>-64</v>
       </c>
       <c r="E129" t="n">
-        <v>-52</v>
+        <v>-63</v>
       </c>
       <c r="F129" t="n">
         <v>-65</v>
@@ -3723,7 +3723,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>7242257600010</t>
+          <t>7228124300018</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
@@ -3732,10 +3732,10 @@
         </is>
       </c>
       <c r="D130" t="n">
-        <v>-62</v>
+        <v>-64</v>
       </c>
       <c r="E130" t="n">
-        <v>-54</v>
+        <v>-63</v>
       </c>
       <c r="F130" t="n">
         <v>-65</v>
@@ -3747,7 +3747,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>7242213400042</t>
+          <t>7228124200069</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
@@ -3759,7 +3759,7 @@
         <v>-54</v>
       </c>
       <c r="E131" t="n">
-        <v>-56</v>
+        <v>-55</v>
       </c>
       <c r="F131" t="n">
         <v>-65</v>
@@ -3771,7 +3771,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>7242218200009</t>
+          <t>7228124300065</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
@@ -3780,10 +3780,10 @@
         </is>
       </c>
       <c r="D132" t="n">
-        <v>-39</v>
+        <v>-56</v>
       </c>
       <c r="E132" t="n">
-        <v>-38</v>
+        <v>-59</v>
       </c>
       <c r="F132" t="n">
         <v>-65</v>
@@ -3795,22 +3795,22 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>7242213600046</t>
+          <t>7228124200007</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D133" t="n">
-        <v/>
+        <v>-59</v>
       </c>
       <c r="E133" t="n">
-        <v/>
+        <v>-58</v>
       </c>
       <c r="F133" t="n">
-        <v/>
+        <v>-65</v>
       </c>
     </row>
     <row r="134">
@@ -3819,7 +3819,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>7242213500013</t>
+          <t>7228124200045</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
@@ -3828,10 +3828,10 @@
         </is>
       </c>
       <c r="D134" t="n">
-        <v>-60</v>
+        <v>-40</v>
       </c>
       <c r="E134" t="n">
-        <v>-57</v>
+        <v>-53</v>
       </c>
       <c r="F134" t="n">
         <v>-65</v>
@@ -3843,7 +3843,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>7242213400003</t>
+          <t>7228124200024</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -3852,10 +3852,10 @@
         </is>
       </c>
       <c r="D135" t="n">
-        <v>-50</v>
+        <v>-59</v>
       </c>
       <c r="E135" t="n">
-        <v>-53</v>
+        <v>-55</v>
       </c>
       <c r="F135" t="n">
         <v>-65</v>
@@ -3867,7 +3867,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>7242218400003</t>
+          <t>7228124200034</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
@@ -3876,10 +3876,10 @@
         </is>
       </c>
       <c r="D136" t="n">
-        <v>-46</v>
+        <v>-60</v>
       </c>
       <c r="E136" t="n">
-        <v>-49</v>
+        <v>-63</v>
       </c>
       <c r="F136" t="n">
         <v>-65</v>
@@ -3891,7 +3891,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>7242218300005</t>
+          <t>7228124200053</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
@@ -3900,10 +3900,10 @@
         </is>
       </c>
       <c r="D137" t="n">
-        <v>-51</v>
+        <v>-58</v>
       </c>
       <c r="E137" t="n">
-        <v>-51</v>
+        <v>-61</v>
       </c>
       <c r="F137" t="n">
         <v>-65</v>
@@ -3915,7 +3915,7 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>7242213400034</t>
+          <t>7228124300040</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
@@ -3924,10 +3924,10 @@
         </is>
       </c>
       <c r="D138" t="n">
-        <v>-47</v>
+        <v>-62</v>
       </c>
       <c r="E138" t="n">
-        <v>-50</v>
+        <v>-64</v>
       </c>
       <c r="F138" t="n">
         <v>-65</v>
@@ -3939,7 +3939,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>7242218300006</t>
+          <t>7228124300042</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
@@ -3948,10 +3948,10 @@
         </is>
       </c>
       <c r="D139" t="n">
-        <v>-51</v>
+        <v>-58</v>
       </c>
       <c r="E139" t="n">
-        <v>-58</v>
+        <v>-61</v>
       </c>
       <c r="F139" t="n">
         <v>-65</v>
@@ -3963,7 +3963,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>7242214000013</t>
+          <t>7228124200027</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
@@ -3972,10 +3972,10 @@
         </is>
       </c>
       <c r="D140" t="n">
-        <v>-57</v>
+        <v>-65</v>
       </c>
       <c r="E140" t="n">
-        <v>-57</v>
+        <v>-59</v>
       </c>
       <c r="F140" t="n">
         <v>-65</v>
@@ -3987,17 +3987,22 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>7242218200040</t>
+          <t>7228124200064</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>PASS</t>
         </is>
       </c>
       <c r="D141" t="n">
-        <v/>
+        <v>-56</v>
       </c>
       <c r="E141" t="n">
-        <v/>
+        <v>-54</v>
       </c>
       <c r="F141" t="n">
-        <v/>
+        <v>-65</v>
       </c>
     </row>
     <row r="142">
@@ -4006,7 +4011,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>7242257600012</t>
+          <t>7228124300051</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
@@ -4018,7 +4023,7 @@
         <v>-64</v>
       </c>
       <c r="E142" t="n">
-        <v>-59</v>
+        <v>-60</v>
       </c>
       <c r="F142" t="n">
         <v>-65</v>
@@ -4030,7 +4035,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>7242213400010</t>
+          <t>7228124300066</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
@@ -4039,10 +4044,10 @@
         </is>
       </c>
       <c r="D143" t="n">
-        <v>-51</v>
+        <v>-59</v>
       </c>
       <c r="E143" t="n">
-        <v>-51</v>
+        <v>-61</v>
       </c>
       <c r="F143" t="n">
         <v>-65</v>
@@ -4054,7 +4059,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>7242218200037</t>
+          <t>7228124200071</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
@@ -4063,12 +4068,204 @@
         </is>
       </c>
       <c r="D144" t="n">
+        <v>-51</v>
+      </c>
+      <c r="E144" t="n">
+        <v>-53</v>
+      </c>
+      <c r="F144" t="n">
+        <v>-65</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="n">
+        <v>144</v>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>7228124200055</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
+      <c r="D145" t="n">
+        <v>-60</v>
+      </c>
+      <c r="E145" t="n">
+        <v>-59</v>
+      </c>
+      <c r="F145" t="n">
+        <v>-65</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="n">
+        <v>145</v>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>7228124200030</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
+      <c r="D146" t="n">
+        <v>-58</v>
+      </c>
+      <c r="E146" t="n">
+        <v>-61</v>
+      </c>
+      <c r="F146" t="n">
+        <v>-65</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="n">
+        <v>146</v>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>7228124300048</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
+      <c r="D147" t="n">
         <v>-57</v>
       </c>
-      <c r="E144" t="n">
-        <v>-58</v>
-      </c>
-      <c r="F144" t="n">
+      <c r="E147" t="n">
+        <v>-59</v>
+      </c>
+      <c r="F147" t="n">
+        <v>-65</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="n">
+        <v>147</v>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>7228124300049</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
+      <c r="D148" t="n">
+        <v>-57</v>
+      </c>
+      <c r="E148" t="n">
+        <v>-62</v>
+      </c>
+      <c r="F148" t="n">
+        <v>-65</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="n">
+        <v>148</v>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>7228124300055</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
+      <c r="D149" t="n">
+        <v>-43</v>
+      </c>
+      <c r="E149" t="n">
+        <v>-43</v>
+      </c>
+      <c r="F149" t="n">
+        <v>-65</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="n">
+        <v>149</v>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>7228124300078</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
+      <c r="D150" t="n">
+        <v>-49</v>
+      </c>
+      <c r="E150" t="n">
+        <v>-50</v>
+      </c>
+      <c r="F150" t="n">
+        <v>-65</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="n">
+        <v>150</v>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>7228124300083</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
+      <c r="D151" t="n">
+        <v>-62</v>
+      </c>
+      <c r="E151" t="n">
+        <v>-59</v>
+      </c>
+      <c r="F151" t="n">
+        <v>-65</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="n">
+        <v>151</v>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>7228124200017</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
+      <c r="D152" t="n">
+        <v>-59</v>
+      </c>
+      <c r="E152" t="n">
+        <v>-57</v>
+      </c>
+      <c r="F152" t="n">
         <v>-65</v>
       </c>
     </row>

</xml_diff>